<commit_message>
Added funding with issuehunt; shields and wechat
</commit_message>
<xml_diff>
--- a/Documentation/Gantt Chart.xlsx
+++ b/Documentation/Gantt Chart.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA71ADEC-D87C-4578-9709-1E4F2C30BAD7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29B5E325-B179-4AAF-BC27-968F2C91932F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectSchedule" sheetId="11" r:id="rId1"/>
@@ -1317,7 +1317,7 @@
     </xf>
     <xf numFmtId="0" fontId="26" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="143">
+  <cellXfs count="144">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1616,12 +1616,100 @@
     <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="10" fontId="27" fillId="6" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="46" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="59" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="60" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="46" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="57" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="58" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="48" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="167" fontId="0" fillId="4" borderId="55" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="4" borderId="53" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="4" borderId="54" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="48" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="31" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="10" fontId="27" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="167" fontId="0" fillId="4" borderId="56" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1631,93 +1719,8 @@
     <xf numFmtId="167" fontId="0" fillId="4" borderId="52" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="4" borderId="54" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="48" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="31" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="46" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="57" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="58" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="48" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="46" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="59" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="60" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="27" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="27" fillId="6" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="14">
@@ -1736,767 +1739,7 @@
     <cellStyle name="Title" xfId="5" builtinId="15" customBuiltin="1"/>
     <cellStyle name="zHiddenText" xfId="3" xr:uid="{26E66EE6-E33F-4D77-BAE4-0FB4F5BBF673}"/>
   </cellStyles>
-  <dxfs count="99">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="darkUp">
-          <fgColor rgb="FF80CA3C"/>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="darkUp">
-          <fgColor rgb="FF80CA3C"/>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="darkUp">
-          <fgColor rgb="FF80CA3C"/>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="darkUp">
-          <fgColor rgb="FF80CA3C"/>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="darkUp">
-          <fgColor rgb="FF80CA3C"/>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="darkUp">
-          <fgColor rgb="FF80CA3C"/>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="darkUp">
-          <fgColor rgb="FF80CA3C"/>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="darkUp">
-          <fgColor rgb="FF80CA3C"/>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="darkUp">
-          <fgColor rgb="FF80CA3C"/>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="darkUp">
-          <fgColor rgb="FF80CA3C"/>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
+  <dxfs count="24">
     <dxf>
       <fill>
         <patternFill>
@@ -2745,15 +1988,15 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="ToDoList" pivot="0" count="9" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="98"/>
-      <tableStyleElement type="headerRow" dxfId="97"/>
-      <tableStyleElement type="totalRow" dxfId="96"/>
-      <tableStyleElement type="firstColumn" dxfId="95"/>
-      <tableStyleElement type="lastColumn" dxfId="94"/>
-      <tableStyleElement type="firstRowStripe" dxfId="93"/>
-      <tableStyleElement type="secondRowStripe" dxfId="92"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="91"/>
-      <tableStyleElement type="secondColumnStripe" dxfId="90"/>
+      <tableStyleElement type="wholeTable" dxfId="23"/>
+      <tableStyleElement type="headerRow" dxfId="22"/>
+      <tableStyleElement type="totalRow" dxfId="21"/>
+      <tableStyleElement type="firstColumn" dxfId="20"/>
+      <tableStyleElement type="lastColumn" dxfId="19"/>
+      <tableStyleElement type="firstRowStripe" dxfId="18"/>
+      <tableStyleElement type="secondRowStripe" dxfId="17"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="16"/>
+      <tableStyleElement type="secondColumnStripe" dxfId="15"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -2824,8 +2067,8 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
     <mruColors>
+      <color rgb="FF80CA3C"/>
       <color rgb="FF8064A2"/>
-      <color rgb="FF80CA3C"/>
       <color rgb="FF6B9D47"/>
       <color rgb="FF80BA4C"/>
       <color rgb="FF86A264"/>
@@ -3173,7 +2416,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q19" sqref="Q19"/>
+      <selection pane="bottomLeft" activeCell="G15" sqref="G15:H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3246,14 +2489,14 @@
       </c>
       <c r="D4" s="107">
         <f ca="1">D5-F4</f>
-        <v>-1.368896925858952E-2</v>
+        <v>-0.1156148282097649</v>
       </c>
       <c r="E4" s="105" t="s">
         <v>54</v>
       </c>
       <c r="F4" s="106">
         <f ca="1">(60-D6)/60</f>
-        <v>0.1</v>
+        <v>0.25</v>
       </c>
       <c r="I4" s="28" t="s">
         <v>15</v>
@@ -3274,7 +2517,7 @@
       </c>
       <c r="D5" s="40">
         <f>SUM(D10,D15)/2</f>
-        <v>8.6311030741410485E-2</v>
+        <v>0.1343851717902351</v>
       </c>
       <c r="E5" s="82" t="s">
         <v>0</v>
@@ -3283,8 +2526,8 @@
         <f>DATE(2020, 6, 15)</f>
         <v>43997</v>
       </c>
-      <c r="G5" s="111"/>
-      <c r="H5" s="111"/>
+      <c r="G5" s="141"/>
+      <c r="H5" s="141"/>
     </row>
     <row r="6" spans="1:69" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A6"/>
@@ -3295,8 +2538,8 @@
         <v>52</v>
       </c>
       <c r="D6" s="41">
-        <f ca="1">DATEDIF(NOW(),BQ7,"D")</f>
-        <v>54</v>
+        <f ca="1">DATEDIF(NOW(),BP7,"D")</f>
+        <v>45</v>
       </c>
       <c r="E6" s="82" t="s">
         <v>6</v>
@@ -3304,107 +2547,107 @@
       <c r="F6" s="84">
         <v>1</v>
       </c>
-      <c r="G6" s="111"/>
-      <c r="H6" s="111"/>
-      <c r="I6" s="112">
+      <c r="G6" s="141"/>
+      <c r="H6" s="141"/>
+      <c r="I6" s="142">
         <f>I7</f>
         <v>43997</v>
       </c>
-      <c r="J6" s="109"/>
-      <c r="K6" s="109"/>
-      <c r="L6" s="109"/>
-      <c r="M6" s="109"/>
-      <c r="N6" s="109"/>
-      <c r="O6" s="113"/>
-      <c r="P6" s="108">
+      <c r="J6" s="130"/>
+      <c r="K6" s="130"/>
+      <c r="L6" s="130"/>
+      <c r="M6" s="130"/>
+      <c r="N6" s="130"/>
+      <c r="O6" s="131"/>
+      <c r="P6" s="129">
         <f>P7</f>
         <v>44004</v>
       </c>
-      <c r="Q6" s="109"/>
-      <c r="R6" s="109"/>
-      <c r="S6" s="109"/>
-      <c r="T6" s="109"/>
-      <c r="U6" s="109"/>
-      <c r="V6" s="113"/>
-      <c r="W6" s="108">
+      <c r="Q6" s="130"/>
+      <c r="R6" s="130"/>
+      <c r="S6" s="130"/>
+      <c r="T6" s="130"/>
+      <c r="U6" s="130"/>
+      <c r="V6" s="131"/>
+      <c r="W6" s="129">
         <f>W7</f>
         <v>44011</v>
       </c>
-      <c r="X6" s="109"/>
-      <c r="Y6" s="109"/>
-      <c r="Z6" s="109"/>
-      <c r="AA6" s="109"/>
-      <c r="AB6" s="109"/>
-      <c r="AC6" s="113"/>
-      <c r="AD6" s="108">
+      <c r="X6" s="130"/>
+      <c r="Y6" s="130"/>
+      <c r="Z6" s="130"/>
+      <c r="AA6" s="130"/>
+      <c r="AB6" s="130"/>
+      <c r="AC6" s="131"/>
+      <c r="AD6" s="129">
         <f>AD7</f>
         <v>44018</v>
       </c>
-      <c r="AE6" s="109"/>
-      <c r="AF6" s="109"/>
-      <c r="AG6" s="109"/>
-      <c r="AH6" s="109"/>
-      <c r="AI6" s="109"/>
-      <c r="AJ6" s="113"/>
-      <c r="AK6" s="108">
+      <c r="AE6" s="130"/>
+      <c r="AF6" s="130"/>
+      <c r="AG6" s="130"/>
+      <c r="AH6" s="130"/>
+      <c r="AI6" s="130"/>
+      <c r="AJ6" s="131"/>
+      <c r="AK6" s="129">
         <f>AK7</f>
         <v>44025</v>
       </c>
-      <c r="AL6" s="109"/>
-      <c r="AM6" s="109"/>
-      <c r="AN6" s="109"/>
-      <c r="AO6" s="109"/>
-      <c r="AP6" s="109"/>
-      <c r="AQ6" s="113"/>
-      <c r="AR6" s="108">
+      <c r="AL6" s="130"/>
+      <c r="AM6" s="130"/>
+      <c r="AN6" s="130"/>
+      <c r="AO6" s="130"/>
+      <c r="AP6" s="130"/>
+      <c r="AQ6" s="131"/>
+      <c r="AR6" s="129">
         <f>AR7</f>
         <v>44032</v>
       </c>
-      <c r="AS6" s="109"/>
-      <c r="AT6" s="109"/>
-      <c r="AU6" s="109"/>
-      <c r="AV6" s="109"/>
-      <c r="AW6" s="109"/>
-      <c r="AX6" s="113"/>
-      <c r="AY6" s="108">
+      <c r="AS6" s="130"/>
+      <c r="AT6" s="130"/>
+      <c r="AU6" s="130"/>
+      <c r="AV6" s="130"/>
+      <c r="AW6" s="130"/>
+      <c r="AX6" s="131"/>
+      <c r="AY6" s="129">
         <f>AY7</f>
         <v>44039</v>
       </c>
-      <c r="AZ6" s="109"/>
-      <c r="BA6" s="109"/>
-      <c r="BB6" s="109"/>
-      <c r="BC6" s="109"/>
-      <c r="BD6" s="109"/>
-      <c r="BE6" s="113"/>
-      <c r="BF6" s="108">
+      <c r="AZ6" s="130"/>
+      <c r="BA6" s="130"/>
+      <c r="BB6" s="130"/>
+      <c r="BC6" s="130"/>
+      <c r="BD6" s="130"/>
+      <c r="BE6" s="131"/>
+      <c r="BF6" s="129">
         <f>BF7</f>
         <v>44046</v>
       </c>
-      <c r="BG6" s="109"/>
-      <c r="BH6" s="109"/>
-      <c r="BI6" s="109"/>
-      <c r="BJ6" s="109"/>
-      <c r="BK6" s="109"/>
-      <c r="BL6" s="113"/>
-      <c r="BM6" s="108">
+      <c r="BG6" s="130"/>
+      <c r="BH6" s="130"/>
+      <c r="BI6" s="130"/>
+      <c r="BJ6" s="130"/>
+      <c r="BK6" s="130"/>
+      <c r="BL6" s="131"/>
+      <c r="BM6" s="129">
         <f>BM7</f>
         <v>44053</v>
       </c>
-      <c r="BN6" s="109"/>
-      <c r="BO6" s="109"/>
-      <c r="BP6" s="109"/>
-      <c r="BQ6" s="110"/>
+      <c r="BN6" s="130"/>
+      <c r="BO6" s="130"/>
+      <c r="BP6" s="130"/>
+      <c r="BQ6" s="140"/>
     </row>
     <row r="7" spans="1:69" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="118"/>
-      <c r="C7" s="118"/>
-      <c r="D7" s="118"/>
-      <c r="E7" s="118"/>
-      <c r="F7" s="118"/>
-      <c r="G7" s="118"/>
+      <c r="B7" s="132"/>
+      <c r="C7" s="132"/>
+      <c r="D7" s="132"/>
+      <c r="E7" s="132"/>
+      <c r="F7" s="132"/>
+      <c r="G7" s="132"/>
       <c r="I7" s="103">
         <f>Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
         <v>43997</v>
@@ -3667,10 +2910,10 @@
       <c r="F8" s="102" t="s">
         <v>4</v>
       </c>
-      <c r="G8" s="121" t="s">
+      <c r="G8" s="135" t="s">
         <v>5</v>
       </c>
-      <c r="H8" s="122"/>
+      <c r="H8" s="136"/>
       <c r="I8" s="9" t="str">
         <f>LEFT(TEXT(I7,"ddd"),1)</f>
         <v>M</v>
@@ -3999,15 +3242,15 @@
       <c r="C10" s="68"/>
       <c r="D10" s="80">
         <f>(D12*DATEDIF(E12,F12,"D")+D13*DATEDIF(E13,F13,"D")+D14*DATEDIF(E14,F14,"D"))/(DATEDIF(E12,F12,"D")+DATEDIF(E13,F13,"D")+DATEDIF(E14,F14,"D"))</f>
-        <v>0.12857142857142856</v>
+        <v>0.17142857142857146</v>
       </c>
       <c r="E10" s="69"/>
       <c r="F10" s="70"/>
-      <c r="G10" s="141">
+      <c r="G10" s="139">
         <f ca="1">DATEDIF(E11,NOW(), "D")/DATEDIF(E11,F14,"d")</f>
-        <v>0.4</v>
-      </c>
-      <c r="H10" s="141"/>
+        <v>0.93333333333333335</v>
+      </c>
+      <c r="H10" s="139"/>
       <c r="I10" s="70"/>
       <c r="J10" s="70"/>
       <c r="K10" s="70"/>
@@ -4072,13 +3315,13 @@
     </row>
     <row r="11" spans="1:69" s="3" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="25"/>
-      <c r="B11" s="135" t="s">
+      <c r="B11" s="113" t="s">
         <v>42</v>
       </c>
-      <c r="C11" s="136"/>
+      <c r="C11" s="114"/>
       <c r="D11" s="64">
         <f ca="1">(60-DATEDIF(NOW(),F11,"D"))/59</f>
-        <v>0.11864406779661017</v>
+        <v>0.25423728813559321</v>
       </c>
       <c r="E11" s="72">
         <f>Project_Start</f>
@@ -4088,11 +3331,11 @@
         <f>E11+59</f>
         <v>44056</v>
       </c>
-      <c r="G11" s="137">
+      <c r="G11" s="115">
         <f t="shared" ref="G11:G22" si="4">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v>60</v>
       </c>
-      <c r="H11" s="138"/>
+      <c r="H11" s="116"/>
       <c r="I11" s="65"/>
       <c r="J11" s="66"/>
       <c r="K11" s="66"/>
@@ -4159,12 +3402,12 @@
       <c r="A12" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="131" t="s">
+      <c r="B12" s="111" t="s">
         <v>53</v>
       </c>
-      <c r="C12" s="132"/>
+      <c r="C12" s="112"/>
       <c r="D12" s="12">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="E12" s="73">
         <f>Project_Start</f>
@@ -4174,15 +3417,15 @@
         <f>E12+6</f>
         <v>44003</v>
       </c>
-      <c r="G12" s="139">
+      <c r="G12" s="117">
         <f t="shared" si="4"/>
         <v>7</v>
       </c>
-      <c r="H12" s="140"/>
+      <c r="H12" s="118"/>
       <c r="I12" s="48"/>
       <c r="J12" s="33"/>
-      <c r="K12" s="33"/>
-      <c r="L12" s="33"/>
+      <c r="K12" s="143"/>
+      <c r="L12" s="143"/>
       <c r="M12" s="33"/>
       <c r="N12" s="33"/>
       <c r="O12" s="33"/>
@@ -4245,10 +3488,10 @@
       <c r="A13" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="131" t="s">
+      <c r="B13" s="111" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="132"/>
+      <c r="C13" s="112"/>
       <c r="D13" s="12">
         <v>0</v>
       </c>
@@ -4260,11 +3503,11 @@
         <f>E13+1</f>
         <v>44005</v>
       </c>
-      <c r="G13" s="139">
+      <c r="G13" s="117">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="H13" s="140"/>
+      <c r="H13" s="118"/>
       <c r="I13" s="47"/>
       <c r="J13" s="33"/>
       <c r="K13" s="33"/>
@@ -4329,10 +3572,10 @@
     </row>
     <row r="14" spans="1:69" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="25"/>
-      <c r="B14" s="129" t="s">
+      <c r="B14" s="123" t="s">
         <v>41</v>
       </c>
-      <c r="C14" s="130"/>
+      <c r="C14" s="124"/>
       <c r="D14" s="50">
         <v>0</v>
       </c>
@@ -4344,11 +3587,11 @@
         <f>E14+7</f>
         <v>44012</v>
       </c>
-      <c r="G14" s="133">
+      <c r="G14" s="109">
         <f t="shared" si="4"/>
         <v>8</v>
       </c>
-      <c r="H14" s="134"/>
+      <c r="H14" s="110"/>
       <c r="I14" s="51"/>
       <c r="J14" s="52"/>
       <c r="K14" s="52"/>
@@ -4421,15 +3664,15 @@
       <c r="C15" s="57"/>
       <c r="D15" s="58">
         <f>(D16*DATEDIF(E16,F16,"D")+D17*DATEDIF(E17,F17,"D")+D18*DATEDIF(E18,F18,"D")+D19*DATEDIF(E19,F19,"D")+D20*DATEDIF(E20,F20,"D")+D21*DATEDIF(E21,F21,"D")+D22*DATEDIF(E22,F22,"D"))/(DATEDIF(E16,F16,"D")+DATEDIF(E17,F17,"D")+DATEDIF(E18,F18,"D")+DATEDIF(E19,F19,"D")+DATEDIF(E20,F20,"D")+DATEDIF(E21,F21,"D")+DATEDIF(E22,F22,"D"))</f>
-        <v>4.4050632911392405E-2</v>
+        <v>9.7341772151898737E-2</v>
       </c>
       <c r="E15" s="59"/>
       <c r="F15" s="60"/>
-      <c r="G15" s="142">
+      <c r="G15" s="108">
         <f ca="1">DATEDIF(E16,NOW(), "D")/DATEDIF(E16,BQ7,"d")</f>
-        <v>8.4745762711864403E-2</v>
-      </c>
-      <c r="H15" s="142"/>
+        <v>0.22033898305084745</v>
+      </c>
+      <c r="H15" s="108"/>
       <c r="I15" s="61"/>
       <c r="J15" s="61"/>
       <c r="K15" s="61"/>
@@ -4494,10 +3737,10 @@
     </row>
     <row r="16" spans="1:69" s="3" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="26"/>
-      <c r="B16" s="127" t="s">
+      <c r="B16" s="121" t="s">
         <v>49</v>
       </c>
-      <c r="C16" s="128"/>
+      <c r="C16" s="122"/>
       <c r="D16" s="54">
         <v>1</v>
       </c>
@@ -4508,11 +3751,11 @@
         <f>E16+1</f>
         <v>43999</v>
       </c>
-      <c r="G16" s="119">
+      <c r="G16" s="133">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="H16" s="120"/>
+      <c r="H16" s="134"/>
       <c r="I16" s="55"/>
       <c r="J16" s="56"/>
       <c r="K16" s="56"/>
@@ -4577,12 +3820,12 @@
     </row>
     <row r="17" spans="1:69" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="26"/>
-      <c r="B17" s="125" t="s">
+      <c r="B17" s="119" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="126"/>
+      <c r="C17" s="120"/>
       <c r="D17" s="13">
-        <v>0.08</v>
+        <v>0.2</v>
       </c>
       <c r="E17" s="79">
         <f>F14-12</f>
@@ -4592,11 +3835,11 @@
         <f>E17+31</f>
         <v>44031</v>
       </c>
-      <c r="G17" s="114">
+      <c r="G17" s="125">
         <f t="shared" si="4"/>
         <v>32</v>
       </c>
-      <c r="H17" s="115"/>
+      <c r="H17" s="126"/>
       <c r="I17" s="49"/>
       <c r="J17" s="35"/>
       <c r="K17" s="35"/>
@@ -4661,12 +3904,12 @@
     </row>
     <row r="18" spans="1:69" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="25"/>
-      <c r="B18" s="125" t="s">
+      <c r="B18" s="119" t="s">
         <v>45</v>
       </c>
-      <c r="C18" s="126"/>
+      <c r="C18" s="120"/>
       <c r="D18" s="13">
-        <v>0</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="E18" s="79">
         <f>F17-7</f>
@@ -4676,11 +3919,11 @@
         <f>E18+7</f>
         <v>44031</v>
       </c>
-      <c r="G18" s="114">
+      <c r="G18" s="125">
         <f t="shared" si="4"/>
         <v>8</v>
       </c>
-      <c r="H18" s="115"/>
+      <c r="H18" s="126"/>
       <c r="I18" s="49"/>
       <c r="J18" s="35"/>
       <c r="K18" s="35"/>
@@ -4745,10 +3988,10 @@
     </row>
     <row r="19" spans="1:69" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="25"/>
-      <c r="B19" s="125" t="s">
+      <c r="B19" s="119" t="s">
         <v>44</v>
       </c>
-      <c r="C19" s="126"/>
+      <c r="C19" s="120"/>
       <c r="D19" s="13">
         <v>0</v>
       </c>
@@ -4760,11 +4003,11 @@
         <f>E19+10</f>
         <v>44034</v>
       </c>
-      <c r="G19" s="114">
+      <c r="G19" s="125">
         <f t="shared" si="4"/>
         <v>11</v>
       </c>
-      <c r="H19" s="115"/>
+      <c r="H19" s="126"/>
       <c r="I19" s="49"/>
       <c r="J19" s="35"/>
       <c r="K19" s="35"/>
@@ -4829,10 +4072,10 @@
     </row>
     <row r="20" spans="1:69" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="25"/>
-      <c r="B20" s="125" t="s">
+      <c r="B20" s="119" t="s">
         <v>48</v>
       </c>
-      <c r="C20" s="126"/>
+      <c r="C20" s="120"/>
       <c r="D20" s="13">
         <v>0</v>
       </c>
@@ -4844,11 +4087,11 @@
         <f>E20+10</f>
         <v>44041</v>
       </c>
-      <c r="G20" s="114">
+      <c r="G20" s="125">
         <f t="shared" si="4"/>
         <v>11</v>
       </c>
-      <c r="H20" s="115"/>
+      <c r="H20" s="126"/>
       <c r="I20" s="49"/>
       <c r="J20" s="35"/>
       <c r="K20" s="35"/>
@@ -4913,10 +4156,10 @@
     </row>
     <row r="21" spans="1:69" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="25"/>
-      <c r="B21" s="125" t="s">
+      <c r="B21" s="119" t="s">
         <v>47</v>
       </c>
-      <c r="C21" s="126"/>
+      <c r="C21" s="120"/>
       <c r="D21" s="13">
         <v>0</v>
       </c>
@@ -4928,11 +4171,11 @@
         <f>E21+10</f>
         <v>44044</v>
       </c>
-      <c r="G21" s="114">
+      <c r="G21" s="125">
         <f t="shared" si="4"/>
         <v>11</v>
       </c>
-      <c r="H21" s="115"/>
+      <c r="H21" s="126"/>
       <c r="I21" s="49"/>
       <c r="J21" s="35"/>
       <c r="K21" s="35"/>
@@ -4997,10 +4240,10 @@
     </row>
     <row r="22" spans="1:69" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="25"/>
-      <c r="B22" s="123" t="s">
+      <c r="B22" s="137" t="s">
         <v>46</v>
       </c>
-      <c r="C22" s="124"/>
+      <c r="C22" s="138"/>
       <c r="D22" s="85">
         <v>0</v>
       </c>
@@ -5012,11 +4255,11 @@
         <f>E22+10</f>
         <v>44047</v>
       </c>
-      <c r="G22" s="116">
+      <c r="G22" s="127">
         <f t="shared" si="4"/>
         <v>11</v>
       </c>
-      <c r="H22" s="117"/>
+      <c r="H22" s="128"/>
       <c r="I22" s="87"/>
       <c r="J22" s="88"/>
       <c r="K22" s="88"/>
@@ -5091,18 +4334,14 @@
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="BM6:BQ6"/>
+    <mergeCell ref="G5:H6"/>
+    <mergeCell ref="I6:O6"/>
+    <mergeCell ref="P6:V6"/>
+    <mergeCell ref="W6:AC6"/>
+    <mergeCell ref="AD6:AJ6"/>
+    <mergeCell ref="AK6:AQ6"/>
     <mergeCell ref="G21:H21"/>
     <mergeCell ref="G22:H22"/>
     <mergeCell ref="AR6:AX6"/>
@@ -5119,14 +4358,18 @@
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="B19:C19"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="BM6:BQ6"/>
-    <mergeCell ref="G5:H6"/>
-    <mergeCell ref="I6:O6"/>
-    <mergeCell ref="P6:V6"/>
-    <mergeCell ref="W6:AC6"/>
-    <mergeCell ref="AD6:AJ6"/>
-    <mergeCell ref="AK6:AQ6"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="G13:H13"/>
   </mergeCells>
   <conditionalFormatting sqref="AF10:AF11 BH10:BH11 D9:D15 D17:D22">
     <cfRule type="dataBar" priority="40">
@@ -5143,15 +4386,15 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I11:BP14 I22:BL22 BM21:BP22 I17:BP21 BQ7:BQ8 I7:BP9">
-    <cfRule type="expression" dxfId="29" priority="59">
+    <cfRule type="expression" dxfId="14" priority="59">
       <formula>AND(TODAY()&gt;=I$7,TODAY()&lt;J$7)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I9:BP9 I11:BP14 I22:BL22 BM21:BP22 I17:BP21">
-    <cfRule type="expression" dxfId="28" priority="53">
+    <cfRule type="expression" dxfId="13" priority="53">
       <formula>AND(task_start&lt;=I$7,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$7)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="54" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="54" stopIfTrue="1">
       <formula>AND(task_end&gt;=I$7,task_start&lt;J$7)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5170,28 +4413,28 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I21:BL21">
-    <cfRule type="expression" dxfId="26" priority="23">
+    <cfRule type="expression" dxfId="11" priority="23">
       <formula>AND(TODAY()&gt;=I$7,TODAY()&lt;J$7)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I21:BL21">
-    <cfRule type="expression" dxfId="25" priority="21">
+    <cfRule type="expression" dxfId="10" priority="21">
       <formula>AND(task_start&lt;=I$7,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$7)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="22" stopIfTrue="1">
       <formula>AND(task_end&gt;=I$7,task_start&lt;J$7)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ9 BQ11:BQ14 BQ17:BQ22">
-    <cfRule type="expression" dxfId="23" priority="61">
+    <cfRule type="expression" dxfId="8" priority="61">
       <formula>AND(TODAY()&gt;=BQ$7,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ9 BQ11:BQ14 BQ17:BQ22">
-    <cfRule type="expression" dxfId="22" priority="64">
+    <cfRule type="expression" dxfId="7" priority="64">
       <formula>AND(task_start&lt;=BQ$7,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=BQ$7)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="65" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="65" stopIfTrue="1">
       <formula>AND(task_end&gt;=BQ$7,task_start&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5210,28 +4453,28 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I16:BP16">
-    <cfRule type="expression" dxfId="20" priority="6">
+    <cfRule type="expression" dxfId="5" priority="6">
       <formula>AND(TODAY()&gt;=I$7,TODAY()&lt;J$7)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ16">
-    <cfRule type="expression" dxfId="19" priority="7">
+    <cfRule type="expression" dxfId="4" priority="7">
       <formula>AND(TODAY()&gt;=BQ$7,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ16">
-    <cfRule type="expression" dxfId="18" priority="8">
+    <cfRule type="expression" dxfId="3" priority="8">
       <formula>AND(task_start&lt;=BQ$7,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=BQ$7)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="9" stopIfTrue="1">
       <formula>AND(task_end&gt;=BQ$7,task_start&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I16:BP16">
-    <cfRule type="expression" dxfId="16" priority="4">
+    <cfRule type="expression" dxfId="1" priority="4">
       <formula>AND(task_start&lt;=I$7,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$7)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="5" stopIfTrue="1">
       <formula>AND(task_end&gt;=I$7,task_start&lt;J$7)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Almost finished main.bas; CD; DFD; gantt.
</commit_message>
<xml_diff>
--- a/Documentation/Gantt Chart.xlsx
+++ b/Documentation/Gantt Chart.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29B5E325-B179-4AAF-BC27-968F2C91932F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9DA341A-719F-4820-8FBF-03319A49157B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="7125" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectSchedule" sheetId="11" r:id="rId1"/>
@@ -25,18 +25,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="55">
   <si>
     <t>Project Start:</t>
   </si>
@@ -224,9 +218,6 @@
   </si>
   <si>
     <t>Questions</t>
-  </si>
-  <si>
-    <t>Actual Time (Excluding allocated time)</t>
   </si>
   <si>
     <t xml:space="preserve">Total:  </t>
@@ -459,7 +450,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -532,18 +523,25 @@
       </patternFill>
     </fill>
     <fill>
-      <patternFill patternType="darkUp">
-        <fgColor rgb="FF80CA3C"/>
-      </patternFill>
-    </fill>
-    <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor rgb="FF80CA3C"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="61">
+  <borders count="70">
     <border>
       <left/>
       <right/>
@@ -941,21 +939,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="dashed">
-        <color theme="0" tint="-0.1498764000366222"/>
-      </left>
-      <right style="dashed">
-        <color theme="0" tint="-0.1498764000366222"/>
-      </right>
-      <top style="medium">
-        <color theme="0" tint="-0.14996795556505021"/>
-      </top>
-      <bottom style="thick">
-        <color theme="0" tint="-0.14996795556505021"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thick">
         <color theme="0" tint="-0.14993743705557422"/>
@@ -1281,6 +1264,120 @@
         <color theme="0" tint="-0.14993743705557422"/>
       </top>
       <bottom style="medium">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </top>
+      <bottom style="medium">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </top>
+      <bottom style="thick">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14990691854609822"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </top>
+      <bottom style="thick">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.14990691854609822"/>
+      </right>
+      <top style="medium">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </top>
+      <bottom style="thick">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.14990691854609822"/>
+      </right>
+      <top style="medium">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </top>
+      <bottom style="thick">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thick">
         <color theme="0" tint="-0.14996795556505021"/>
       </bottom>
       <diagonal/>
@@ -1317,7 +1414,7 @@
     </xf>
     <xf numFmtId="0" fontId="26" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="144">
+  <cellXfs count="168">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1427,14 +1524,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="26" fillId="11" borderId="5" xfId="13" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1455,9 +1551,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="4" fillId="3" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1554,56 +1647,53 @@
     <xf numFmtId="9" fontId="4" fillId="3" borderId="31" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="7" fillId="3" borderId="32" xfId="10" applyNumberFormat="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="9" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="26" fillId="11" borderId="36" xfId="13" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="11" borderId="37" xfId="13" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="26" fillId="5" borderId="38" xfId="13" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="13" borderId="39" xfId="13" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="9" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="26" fillId="11" borderId="37" xfId="13" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="11" borderId="38" xfId="13" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="26" fillId="5" borderId="39" xfId="13" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="14" borderId="40" xfId="13" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="13" borderId="40" xfId="13" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="14" borderId="41" xfId="13" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="26" fillId="6" borderId="41" xfId="13" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="13" borderId="42" xfId="13" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="26" fillId="6" borderId="42" xfId="13" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="14" borderId="43" xfId="13" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="9" fillId="4" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="9" fillId="4" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="168" fontId="26" fillId="11" borderId="0" xfId="13" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1616,27 +1706,94 @@
     <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="27" fillId="6" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="46" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="167" fontId="0" fillId="4" borderId="54" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="4" borderId="52" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="4" borderId="55" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="4" borderId="51" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="4" borderId="53" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="47" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="31" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="45" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="56" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="57" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="47" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="45" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
+    <xf numFmtId="10" fontId="27" fillId="6" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="58" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="59" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="60" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1649,77 +1806,87 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="46" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="57" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="58" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="48" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="4" borderId="55" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="4" borderId="53" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="4" borderId="54" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="48" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="31" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="10" fontId="27" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="4" borderId="56" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="4" borderId="52" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="27" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="7" fillId="3" borderId="24" xfId="10" applyNumberFormat="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="7" fillId="3" borderId="27" xfId="10" applyNumberFormat="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="60" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="60" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="61" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="62" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="6" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="63" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="64" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="65" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="66" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="67" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="67" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="68" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="60" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="69" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2067,8 +2234,8 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
     <mruColors>
+      <color rgb="FF8064A2"/>
       <color rgb="FF80CA3C"/>
-      <color rgb="FF8064A2"/>
       <color rgb="FF6B9D47"/>
       <color rgb="FF80BA4C"/>
       <color rgb="FF86A264"/>
@@ -2416,7 +2583,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G15" sqref="G15:H15"/>
+      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2433,7 +2600,13 @@
     <col min="65" max="69" width="2.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:69" ht="9.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1" spans="1:69" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU1" s="144"/>
+      <c r="AV1" s="144"/>
+      <c r="AW1" s="144"/>
+      <c r="AX1" s="144"/>
+      <c r="AY1" s="144"/>
+    </row>
     <row r="2" spans="1:69" ht="24.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="26" t="s">
         <v>24</v>
@@ -2457,11 +2630,11 @@
       <c r="AN2" t="s">
         <v>38</v>
       </c>
-      <c r="AW2" s="43"/>
-      <c r="AX2" s="43"/>
-      <c r="AY2" t="s">
-        <v>50</v>
-      </c>
+      <c r="AU2" s="144"/>
+      <c r="AV2" s="144"/>
+      <c r="AW2" s="145"/>
+      <c r="AX2" s="145"/>
+      <c r="AY2" s="144"/>
     </row>
     <row r="3" spans="1:69" ht="3" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="26"/>
@@ -2474,8 +2647,11 @@
       <c r="I3" s="10"/>
       <c r="AL3" s="37"/>
       <c r="AM3" s="32"/>
-      <c r="AW3" s="43"/>
-      <c r="AX3" s="43"/>
+      <c r="AU3" s="144"/>
+      <c r="AV3" s="144"/>
+      <c r="AW3" s="145"/>
+      <c r="AX3" s="145"/>
+      <c r="AY3" s="144"/>
     </row>
     <row r="4" spans="1:69" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="25" t="s">
@@ -2485,18 +2661,18 @@
         <v>34</v>
       </c>
       <c r="C4" s="38" t="s">
-        <v>55</v>
-      </c>
-      <c r="D4" s="107">
+        <v>54</v>
+      </c>
+      <c r="D4" s="104">
         <f ca="1">D5-F4</f>
-        <v>-0.1156148282097649</v>
-      </c>
-      <c r="E4" s="105" t="s">
-        <v>54</v>
-      </c>
-      <c r="F4" s="106">
+        <v>-0.45503144654088046</v>
+      </c>
+      <c r="E4" s="102" t="s">
+        <v>53</v>
+      </c>
+      <c r="F4" s="103">
         <f ca="1">(60-D6)/60</f>
-        <v>0.25</v>
+        <v>0.98333333333333328</v>
       </c>
       <c r="I4" s="28" t="s">
         <v>15</v>
@@ -2506,6 +2682,11 @@
       <c r="AN4" t="s">
         <v>39</v>
       </c>
+      <c r="AU4" s="144"/>
+      <c r="AV4" s="144"/>
+      <c r="AW4" s="144"/>
+      <c r="AX4" s="144"/>
+      <c r="AY4" s="144"/>
     </row>
     <row r="5" spans="1:69" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5"/>
@@ -2513,21 +2694,21 @@
         <v>25</v>
       </c>
       <c r="C5" s="39" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D5" s="40">
         <f>SUM(D10,D15)/2</f>
-        <v>0.1343851717902351</v>
-      </c>
-      <c r="E5" s="82" t="s">
+        <v>0.52830188679245282</v>
+      </c>
+      <c r="E5" s="80" t="s">
         <v>0</v>
       </c>
-      <c r="F5" s="83">
+      <c r="F5" s="81">
         <f>DATE(2020, 6, 15)</f>
         <v>43997</v>
       </c>
-      <c r="G5" s="141"/>
-      <c r="H5" s="141"/>
+      <c r="G5" s="108"/>
+      <c r="H5" s="108"/>
     </row>
     <row r="6" spans="1:69" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A6"/>
@@ -2535,140 +2716,140 @@
         <v>26</v>
       </c>
       <c r="C6" s="38" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D6" s="41">
         <f ca="1">DATEDIF(NOW(),BP7,"D")</f>
-        <v>45</v>
-      </c>
-      <c r="E6" s="82" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="80" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="84">
+      <c r="F6" s="82">
         <v>1</v>
       </c>
-      <c r="G6" s="141"/>
-      <c r="H6" s="141"/>
-      <c r="I6" s="142">
+      <c r="G6" s="108"/>
+      <c r="H6" s="108"/>
+      <c r="I6" s="109">
         <f>I7</f>
         <v>43997</v>
       </c>
-      <c r="J6" s="130"/>
-      <c r="K6" s="130"/>
-      <c r="L6" s="130"/>
-      <c r="M6" s="130"/>
-      <c r="N6" s="130"/>
-      <c r="O6" s="131"/>
-      <c r="P6" s="129">
+      <c r="J6" s="106"/>
+      <c r="K6" s="106"/>
+      <c r="L6" s="106"/>
+      <c r="M6" s="106"/>
+      <c r="N6" s="106"/>
+      <c r="O6" s="110"/>
+      <c r="P6" s="105">
         <f>P7</f>
         <v>44004</v>
       </c>
-      <c r="Q6" s="130"/>
-      <c r="R6" s="130"/>
-      <c r="S6" s="130"/>
-      <c r="T6" s="130"/>
-      <c r="U6" s="130"/>
-      <c r="V6" s="131"/>
-      <c r="W6" s="129">
+      <c r="Q6" s="106"/>
+      <c r="R6" s="106"/>
+      <c r="S6" s="106"/>
+      <c r="T6" s="106"/>
+      <c r="U6" s="106"/>
+      <c r="V6" s="110"/>
+      <c r="W6" s="105">
         <f>W7</f>
         <v>44011</v>
       </c>
-      <c r="X6" s="130"/>
-      <c r="Y6" s="130"/>
-      <c r="Z6" s="130"/>
-      <c r="AA6" s="130"/>
-      <c r="AB6" s="130"/>
-      <c r="AC6" s="131"/>
-      <c r="AD6" s="129">
+      <c r="X6" s="106"/>
+      <c r="Y6" s="106"/>
+      <c r="Z6" s="106"/>
+      <c r="AA6" s="106"/>
+      <c r="AB6" s="106"/>
+      <c r="AC6" s="110"/>
+      <c r="AD6" s="105">
         <f>AD7</f>
         <v>44018</v>
       </c>
-      <c r="AE6" s="130"/>
-      <c r="AF6" s="130"/>
-      <c r="AG6" s="130"/>
-      <c r="AH6" s="130"/>
-      <c r="AI6" s="130"/>
-      <c r="AJ6" s="131"/>
-      <c r="AK6" s="129">
+      <c r="AE6" s="106"/>
+      <c r="AF6" s="106"/>
+      <c r="AG6" s="106"/>
+      <c r="AH6" s="106"/>
+      <c r="AI6" s="106"/>
+      <c r="AJ6" s="110"/>
+      <c r="AK6" s="105">
         <f>AK7</f>
         <v>44025</v>
       </c>
-      <c r="AL6" s="130"/>
-      <c r="AM6" s="130"/>
-      <c r="AN6" s="130"/>
-      <c r="AO6" s="130"/>
-      <c r="AP6" s="130"/>
-      <c r="AQ6" s="131"/>
-      <c r="AR6" s="129">
+      <c r="AL6" s="106"/>
+      <c r="AM6" s="106"/>
+      <c r="AN6" s="106"/>
+      <c r="AO6" s="106"/>
+      <c r="AP6" s="106"/>
+      <c r="AQ6" s="110"/>
+      <c r="AR6" s="105">
         <f>AR7</f>
         <v>44032</v>
       </c>
-      <c r="AS6" s="130"/>
-      <c r="AT6" s="130"/>
-      <c r="AU6" s="130"/>
-      <c r="AV6" s="130"/>
-      <c r="AW6" s="130"/>
-      <c r="AX6" s="131"/>
-      <c r="AY6" s="129">
+      <c r="AS6" s="106"/>
+      <c r="AT6" s="106"/>
+      <c r="AU6" s="106"/>
+      <c r="AV6" s="106"/>
+      <c r="AW6" s="106"/>
+      <c r="AX6" s="110"/>
+      <c r="AY6" s="105">
         <f>AY7</f>
         <v>44039</v>
       </c>
-      <c r="AZ6" s="130"/>
-      <c r="BA6" s="130"/>
-      <c r="BB6" s="130"/>
-      <c r="BC6" s="130"/>
-      <c r="BD6" s="130"/>
-      <c r="BE6" s="131"/>
-      <c r="BF6" s="129">
+      <c r="AZ6" s="106"/>
+      <c r="BA6" s="106"/>
+      <c r="BB6" s="106"/>
+      <c r="BC6" s="106"/>
+      <c r="BD6" s="106"/>
+      <c r="BE6" s="110"/>
+      <c r="BF6" s="105">
         <f>BF7</f>
         <v>44046</v>
       </c>
-      <c r="BG6" s="130"/>
-      <c r="BH6" s="130"/>
-      <c r="BI6" s="130"/>
-      <c r="BJ6" s="130"/>
-      <c r="BK6" s="130"/>
-      <c r="BL6" s="131"/>
-      <c r="BM6" s="129">
+      <c r="BG6" s="106"/>
+      <c r="BH6" s="106"/>
+      <c r="BI6" s="106"/>
+      <c r="BJ6" s="106"/>
+      <c r="BK6" s="106"/>
+      <c r="BL6" s="110"/>
+      <c r="BM6" s="105">
         <f>BM7</f>
         <v>44053</v>
       </c>
-      <c r="BN6" s="130"/>
-      <c r="BO6" s="130"/>
-      <c r="BP6" s="130"/>
-      <c r="BQ6" s="140"/>
+      <c r="BN6" s="106"/>
+      <c r="BO6" s="106"/>
+      <c r="BP6" s="106"/>
+      <c r="BQ6" s="107"/>
     </row>
     <row r="7" spans="1:69" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="132"/>
-      <c r="C7" s="132"/>
-      <c r="D7" s="132"/>
-      <c r="E7" s="132"/>
-      <c r="F7" s="132"/>
-      <c r="G7" s="132"/>
-      <c r="I7" s="103">
+      <c r="B7" s="115"/>
+      <c r="C7" s="115"/>
+      <c r="D7" s="115"/>
+      <c r="E7" s="115"/>
+      <c r="F7" s="115"/>
+      <c r="G7" s="115"/>
+      <c r="I7" s="100">
         <f>Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
         <v>43997</v>
       </c>
-      <c r="J7" s="90">
+      <c r="J7" s="87">
         <f>I7+1</f>
         <v>43998</v>
       </c>
-      <c r="K7" s="90">
+      <c r="K7" s="87">
         <f t="shared" ref="K7:AX7" si="0">J7+1</f>
         <v>43999</v>
       </c>
-      <c r="L7" s="90">
+      <c r="L7" s="87">
         <f t="shared" si="0"/>
         <v>44000</v>
       </c>
-      <c r="M7" s="90">
+      <c r="M7" s="87">
         <f t="shared" si="0"/>
         <v>44001</v>
       </c>
-      <c r="N7" s="90">
+      <c r="N7" s="87">
         <f t="shared" si="0"/>
         <v>44002</v>
       </c>
@@ -2680,23 +2861,23 @@
         <f>O7+1</f>
         <v>44004</v>
       </c>
-      <c r="Q7" s="90">
+      <c r="Q7" s="87">
         <f>P7+1</f>
         <v>44005</v>
       </c>
-      <c r="R7" s="90">
+      <c r="R7" s="87">
         <f t="shared" si="0"/>
         <v>44006</v>
       </c>
-      <c r="S7" s="90">
+      <c r="S7" s="87">
         <f t="shared" si="0"/>
         <v>44007</v>
       </c>
-      <c r="T7" s="90">
+      <c r="T7" s="87">
         <f t="shared" si="0"/>
         <v>44008</v>
       </c>
-      <c r="U7" s="90">
+      <c r="U7" s="87">
         <f t="shared" si="0"/>
         <v>44009</v>
       </c>
@@ -2708,23 +2889,23 @@
         <f>V7+1</f>
         <v>44011</v>
       </c>
-      <c r="X7" s="90">
+      <c r="X7" s="87">
         <f>W7+1</f>
         <v>44012</v>
       </c>
-      <c r="Y7" s="104">
+      <c r="Y7" s="101">
         <f>X7+1</f>
         <v>44013</v>
       </c>
-      <c r="Z7" s="90">
+      <c r="Z7" s="87">
         <f t="shared" si="0"/>
         <v>44014</v>
       </c>
-      <c r="AA7" s="90">
+      <c r="AA7" s="87">
         <f t="shared" si="0"/>
         <v>44015</v>
       </c>
-      <c r="AB7" s="90">
+      <c r="AB7" s="87">
         <f t="shared" si="0"/>
         <v>44016</v>
       </c>
@@ -2736,23 +2917,23 @@
         <f>AC7+1</f>
         <v>44018</v>
       </c>
-      <c r="AE7" s="90">
+      <c r="AE7" s="87">
         <f>AD7+1</f>
         <v>44019</v>
       </c>
-      <c r="AF7" s="90">
+      <c r="AF7" s="87">
         <f t="shared" si="0"/>
         <v>44020</v>
       </c>
-      <c r="AG7" s="90">
+      <c r="AG7" s="87">
         <f t="shared" si="0"/>
         <v>44021</v>
       </c>
-      <c r="AH7" s="90">
+      <c r="AH7" s="87">
         <f t="shared" si="0"/>
         <v>44022</v>
       </c>
-      <c r="AI7" s="90">
+      <c r="AI7" s="87">
         <f t="shared" si="0"/>
         <v>44023</v>
       </c>
@@ -2764,23 +2945,23 @@
         <f>AJ7+1</f>
         <v>44025</v>
       </c>
-      <c r="AL7" s="90">
+      <c r="AL7" s="87">
         <f>AK7+1</f>
         <v>44026</v>
       </c>
-      <c r="AM7" s="90">
+      <c r="AM7" s="87">
         <f t="shared" si="0"/>
         <v>44027</v>
       </c>
-      <c r="AN7" s="90">
+      <c r="AN7" s="87">
         <f t="shared" si="0"/>
         <v>44028</v>
       </c>
-      <c r="AO7" s="90">
+      <c r="AO7" s="87">
         <f t="shared" si="0"/>
         <v>44029</v>
       </c>
-      <c r="AP7" s="90">
+      <c r="AP7" s="87">
         <f t="shared" si="0"/>
         <v>44030</v>
       </c>
@@ -2792,23 +2973,23 @@
         <f>AQ7+1</f>
         <v>44032</v>
       </c>
-      <c r="AS7" s="90">
+      <c r="AS7" s="87">
         <f>AR7+1</f>
         <v>44033</v>
       </c>
-      <c r="AT7" s="90">
+      <c r="AT7" s="87">
         <f t="shared" si="0"/>
         <v>44034</v>
       </c>
-      <c r="AU7" s="90">
+      <c r="AU7" s="87">
         <f t="shared" si="0"/>
         <v>44035</v>
       </c>
-      <c r="AV7" s="90">
+      <c r="AV7" s="87">
         <f t="shared" si="0"/>
         <v>44036</v>
       </c>
-      <c r="AW7" s="90">
+      <c r="AW7" s="87">
         <f t="shared" si="0"/>
         <v>44037</v>
       </c>
@@ -2820,23 +3001,23 @@
         <f t="shared" ref="AY7:BQ7" si="1">AX7+1</f>
         <v>44039</v>
       </c>
-      <c r="AZ7" s="90">
+      <c r="AZ7" s="87">
         <f t="shared" si="1"/>
         <v>44040</v>
       </c>
-      <c r="BA7" s="90">
+      <c r="BA7" s="87">
         <f t="shared" si="1"/>
         <v>44041</v>
       </c>
-      <c r="BB7" s="90">
+      <c r="BB7" s="87">
         <f t="shared" si="1"/>
         <v>44042</v>
       </c>
-      <c r="BC7" s="90">
+      <c r="BC7" s="87">
         <f t="shared" si="1"/>
         <v>44043</v>
       </c>
-      <c r="BD7" s="90">
+      <c r="BD7" s="87">
         <f t="shared" si="1"/>
         <v>44044</v>
       </c>
@@ -2848,23 +3029,23 @@
         <f t="shared" si="1"/>
         <v>44046</v>
       </c>
-      <c r="BG7" s="90">
+      <c r="BG7" s="87">
         <f t="shared" si="1"/>
         <v>44047</v>
       </c>
-      <c r="BH7" s="90">
+      <c r="BH7" s="87">
         <f t="shared" si="1"/>
         <v>44048</v>
       </c>
-      <c r="BI7" s="90">
+      <c r="BI7" s="87">
         <f t="shared" si="1"/>
         <v>44049</v>
       </c>
-      <c r="BJ7" s="90">
+      <c r="BJ7" s="87">
         <f t="shared" si="1"/>
         <v>44050</v>
       </c>
-      <c r="BK7" s="90">
+      <c r="BK7" s="87">
         <f t="shared" si="1"/>
         <v>44051</v>
       </c>
@@ -2876,19 +3057,19 @@
         <f t="shared" si="1"/>
         <v>44053</v>
       </c>
-      <c r="BN7" s="90">
+      <c r="BN7" s="87">
         <f t="shared" si="1"/>
         <v>44054</v>
       </c>
-      <c r="BO7" s="90">
+      <c r="BO7" s="87">
         <f t="shared" si="1"/>
         <v>44055</v>
       </c>
-      <c r="BP7" s="90">
+      <c r="BP7" s="87">
         <f t="shared" si="1"/>
         <v>44056</v>
       </c>
-      <c r="BQ7" s="91">
+      <c r="BQ7" s="88">
         <f t="shared" si="1"/>
         <v>44057</v>
       </c>
@@ -2897,23 +3078,23 @@
       <c r="A8" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="101" t="s">
+      <c r="B8" s="98" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="102"/>
-      <c r="D8" s="102" t="s">
+      <c r="C8" s="99"/>
+      <c r="D8" s="99" t="s">
         <v>1</v>
       </c>
-      <c r="E8" s="102" t="s">
+      <c r="E8" s="99" t="s">
         <v>3</v>
       </c>
-      <c r="F8" s="102" t="s">
+      <c r="F8" s="99" t="s">
         <v>4</v>
       </c>
-      <c r="G8" s="135" t="s">
+      <c r="G8" s="118" t="s">
         <v>5</v>
       </c>
-      <c r="H8" s="136"/>
+      <c r="H8" s="119"/>
       <c r="I8" s="9" t="str">
         <f>LEFT(TEXT(I7,"ddd"),1)</f>
         <v>M</v>
@@ -2978,7 +3159,7 @@
         <f t="shared" si="2"/>
         <v>T</v>
       </c>
-      <c r="Y8" s="44" t="str">
+      <c r="Y8" s="43" t="str">
         <f>LEFT(TEXT(Y7,"ddd"),1)</f>
         <v>W</v>
       </c>
@@ -3154,7 +3335,7 @@
         <f>LEFT(TEXT(BP7,"ddd"),1)</f>
         <v>T</v>
       </c>
-      <c r="BQ8" s="92" t="str">
+      <c r="BQ8" s="89" t="str">
         <f>LEFT(TEXT(BQ7,"ddd"),1)</f>
         <v>F</v>
       </c>
@@ -3163,268 +3344,265 @@
       <c r="A9" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="98"/>
+      <c r="B9" s="95"/>
       <c r="C9" s="29"/>
       <c r="E9"/>
       <c r="H9" t="str">
         <f>IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v/>
       </c>
-      <c r="I9" s="63"/>
-      <c r="J9" s="63"/>
-      <c r="K9" s="63"/>
-      <c r="L9" s="63"/>
-      <c r="M9" s="63"/>
-      <c r="N9" s="63"/>
-      <c r="O9" s="63"/>
-      <c r="P9" s="63"/>
-      <c r="Q9" s="63"/>
-      <c r="R9" s="63"/>
-      <c r="S9" s="63"/>
-      <c r="T9" s="63"/>
-      <c r="U9" s="63"/>
-      <c r="V9" s="63"/>
-      <c r="W9" s="63"/>
-      <c r="X9" s="63"/>
-      <c r="Y9" s="63"/>
-      <c r="Z9" s="63"/>
-      <c r="AA9" s="63"/>
-      <c r="AB9" s="63"/>
-      <c r="AC9" s="63"/>
-      <c r="AD9" s="63"/>
-      <c r="AE9" s="63"/>
-      <c r="AF9" s="63"/>
-      <c r="AG9" s="63"/>
-      <c r="AH9" s="63"/>
-      <c r="AI9" s="63"/>
-      <c r="AJ9" s="63"/>
-      <c r="AK9" s="63"/>
-      <c r="AL9" s="63"/>
-      <c r="AM9" s="63"/>
-      <c r="AN9" s="63"/>
-      <c r="AO9" s="63"/>
-      <c r="AP9" s="63"/>
-      <c r="AQ9" s="63"/>
-      <c r="AR9" s="63"/>
-      <c r="AS9" s="63"/>
-      <c r="AT9" s="63"/>
-      <c r="AU9" s="63"/>
-      <c r="AV9" s="63"/>
-      <c r="AW9" s="63"/>
-      <c r="AX9" s="63"/>
-      <c r="AY9" s="63"/>
-      <c r="AZ9" s="63"/>
-      <c r="BA9" s="63"/>
-      <c r="BB9" s="63"/>
-      <c r="BC9" s="63"/>
-      <c r="BD9" s="63"/>
-      <c r="BE9" s="63"/>
-      <c r="BF9" s="63"/>
-      <c r="BG9" s="63"/>
-      <c r="BH9" s="63"/>
-      <c r="BI9" s="63"/>
-      <c r="BJ9" s="63"/>
-      <c r="BK9" s="63"/>
-      <c r="BL9" s="63"/>
-      <c r="BM9" s="63"/>
-      <c r="BN9" s="63"/>
-      <c r="BO9" s="63"/>
-      <c r="BP9" s="63"/>
-      <c r="BQ9" s="45"/>
+      <c r="I9" s="61"/>
+      <c r="J9" s="61"/>
+      <c r="K9" s="61"/>
+      <c r="L9" s="61"/>
+      <c r="M9" s="61"/>
+      <c r="N9" s="61"/>
+      <c r="O9" s="61"/>
+      <c r="P9" s="61"/>
+      <c r="Q9" s="61"/>
+      <c r="R9" s="61"/>
+      <c r="S9" s="61"/>
+      <c r="T9" s="61"/>
+      <c r="U9" s="61"/>
+      <c r="V9" s="61"/>
+      <c r="W9" s="61"/>
+      <c r="X9" s="61"/>
+      <c r="Y9" s="61"/>
+      <c r="Z9" s="61"/>
+      <c r="AA9" s="61"/>
+      <c r="AB9" s="61"/>
+      <c r="AC9" s="61"/>
+      <c r="AD9" s="61"/>
+      <c r="AE9" s="61"/>
+      <c r="AF9" s="61"/>
+      <c r="AG9" s="61"/>
+      <c r="AH9" s="61"/>
+      <c r="AI9" s="61"/>
+      <c r="AJ9" s="61"/>
+      <c r="AK9" s="61"/>
+      <c r="AL9" s="61"/>
+      <c r="AM9" s="61"/>
+      <c r="AN9" s="61"/>
+      <c r="AO9" s="61"/>
+      <c r="AP9" s="61"/>
+      <c r="AQ9" s="61"/>
+      <c r="AR9" s="61"/>
+      <c r="AS9" s="61"/>
+      <c r="AT9" s="61"/>
+      <c r="AU9" s="61"/>
+      <c r="AV9" s="61"/>
+      <c r="AW9" s="61"/>
+      <c r="AX9" s="61"/>
+      <c r="AY9" s="61"/>
+      <c r="AZ9" s="61"/>
+      <c r="BA9" s="61"/>
+      <c r="BB9" s="61"/>
+      <c r="BC9" s="61"/>
+      <c r="BD9" s="61"/>
+      <c r="BE9" s="61"/>
+      <c r="BF9" s="61"/>
+      <c r="BG9" s="61"/>
+      <c r="BH9" s="61"/>
+      <c r="BI9" s="61"/>
+      <c r="BJ9" s="61"/>
+      <c r="BK9" s="61"/>
+      <c r="BL9" s="61"/>
+      <c r="BM9" s="61"/>
+      <c r="BN9" s="61"/>
+      <c r="BO9" s="61"/>
+      <c r="BP9" s="61"/>
+      <c r="BQ9" s="44"/>
     </row>
     <row r="10" spans="1:69" s="3" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="99" t="s">
+      <c r="B10" s="96" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="68"/>
-      <c r="D10" s="80">
+      <c r="C10" s="66"/>
+      <c r="D10" s="78">
         <f>(D12*DATEDIF(E12,F12,"D")+D13*DATEDIF(E13,F13,"D")+D14*DATEDIF(E14,F14,"D"))/(DATEDIF(E12,F12,"D")+DATEDIF(E13,F13,"D")+DATEDIF(E14,F14,"D"))</f>
-        <v>0.17142857142857146</v>
-      </c>
-      <c r="E10" s="69"/>
-      <c r="F10" s="70"/>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="E10" s="67"/>
+      <c r="F10" s="68"/>
       <c r="G10" s="139">
-        <f ca="1">DATEDIF(E11,NOW(), "D")/DATEDIF(E11,F14,"d")</f>
-        <v>0.93333333333333335</v>
+        <v>1</v>
       </c>
       <c r="H10" s="139"/>
-      <c r="I10" s="70"/>
-      <c r="J10" s="70"/>
-      <c r="K10" s="70"/>
-      <c r="L10" s="70"/>
-      <c r="M10" s="70"/>
-      <c r="N10" s="70"/>
-      <c r="O10" s="70"/>
-      <c r="P10" s="70"/>
-      <c r="Q10" s="70"/>
-      <c r="R10" s="70"/>
-      <c r="S10" s="70"/>
-      <c r="T10" s="70"/>
-      <c r="U10" s="70"/>
-      <c r="V10" s="70"/>
-      <c r="W10" s="70"/>
-      <c r="X10" s="70"/>
-      <c r="Y10" s="70"/>
-      <c r="Z10" s="70"/>
-      <c r="AA10" s="70"/>
-      <c r="AB10" s="70"/>
-      <c r="AC10" s="70"/>
-      <c r="AD10" s="70"/>
-      <c r="AE10" s="68"/>
-      <c r="AF10" s="71"/>
-      <c r="AG10" s="69"/>
-      <c r="AH10" s="70"/>
-      <c r="AI10" s="70"/>
-      <c r="AJ10" s="70"/>
-      <c r="AK10" s="70"/>
-      <c r="AL10" s="70"/>
-      <c r="AM10" s="70"/>
-      <c r="AN10" s="70"/>
-      <c r="AO10" s="70"/>
-      <c r="AP10" s="70"/>
-      <c r="AQ10" s="70"/>
-      <c r="AR10" s="70"/>
-      <c r="AS10" s="70"/>
-      <c r="AT10" s="70"/>
-      <c r="AU10" s="70"/>
-      <c r="AV10" s="70"/>
-      <c r="AW10" s="70"/>
-      <c r="AX10" s="70"/>
-      <c r="AY10" s="70"/>
-      <c r="AZ10" s="70"/>
-      <c r="BA10" s="70"/>
-      <c r="BB10" s="70"/>
-      <c r="BC10" s="70"/>
-      <c r="BD10" s="70"/>
-      <c r="BE10" s="70"/>
-      <c r="BF10" s="70"/>
-      <c r="BG10" s="68"/>
-      <c r="BH10" s="71"/>
-      <c r="BI10" s="69"/>
-      <c r="BJ10" s="70"/>
-      <c r="BK10" s="70"/>
-      <c r="BL10" s="70"/>
-      <c r="BM10" s="70"/>
-      <c r="BN10" s="70"/>
-      <c r="BO10" s="70"/>
-      <c r="BP10" s="70"/>
-      <c r="BQ10" s="93"/>
+      <c r="I10" s="68"/>
+      <c r="J10" s="68"/>
+      <c r="K10" s="68"/>
+      <c r="L10" s="68"/>
+      <c r="M10" s="68"/>
+      <c r="N10" s="68"/>
+      <c r="O10" s="68"/>
+      <c r="P10" s="68"/>
+      <c r="Q10" s="68"/>
+      <c r="R10" s="68"/>
+      <c r="S10" s="68"/>
+      <c r="T10" s="68"/>
+      <c r="U10" s="68"/>
+      <c r="V10" s="68"/>
+      <c r="W10" s="68"/>
+      <c r="X10" s="68"/>
+      <c r="Y10" s="68"/>
+      <c r="Z10" s="68"/>
+      <c r="AA10" s="68"/>
+      <c r="AB10" s="68"/>
+      <c r="AC10" s="68"/>
+      <c r="AD10" s="68"/>
+      <c r="AE10" s="66"/>
+      <c r="AF10" s="69"/>
+      <c r="AG10" s="67"/>
+      <c r="AH10" s="68"/>
+      <c r="AI10" s="68"/>
+      <c r="AJ10" s="68"/>
+      <c r="AK10" s="68"/>
+      <c r="AL10" s="68"/>
+      <c r="AM10" s="68"/>
+      <c r="AN10" s="68"/>
+      <c r="AO10" s="68"/>
+      <c r="AP10" s="68"/>
+      <c r="AQ10" s="68"/>
+      <c r="AR10" s="68"/>
+      <c r="AS10" s="68"/>
+      <c r="AT10" s="68"/>
+      <c r="AU10" s="68"/>
+      <c r="AV10" s="68"/>
+      <c r="AW10" s="68"/>
+      <c r="AX10" s="68"/>
+      <c r="AY10" s="68"/>
+      <c r="AZ10" s="68"/>
+      <c r="BA10" s="68"/>
+      <c r="BB10" s="68"/>
+      <c r="BC10" s="68"/>
+      <c r="BD10" s="68"/>
+      <c r="BE10" s="68"/>
+      <c r="BF10" s="68"/>
+      <c r="BG10" s="66"/>
+      <c r="BH10" s="69"/>
+      <c r="BI10" s="67"/>
+      <c r="BJ10" s="68"/>
+      <c r="BK10" s="68"/>
+      <c r="BL10" s="68"/>
+      <c r="BM10" s="68"/>
+      <c r="BN10" s="68"/>
+      <c r="BO10" s="68"/>
+      <c r="BP10" s="68"/>
+      <c r="BQ10" s="90"/>
     </row>
     <row r="11" spans="1:69" s="3" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="25"/>
-      <c r="B11" s="113" t="s">
+      <c r="B11" s="133" t="s">
         <v>42</v>
       </c>
-      <c r="C11" s="114"/>
-      <c r="D11" s="64">
+      <c r="C11" s="134"/>
+      <c r="D11" s="62">
         <f ca="1">(60-DATEDIF(NOW(),F11,"D"))/59</f>
-        <v>0.25423728813559321</v>
-      </c>
-      <c r="E11" s="72">
+        <v>1</v>
+      </c>
+      <c r="E11" s="70">
         <f>Project_Start</f>
         <v>43997</v>
       </c>
-      <c r="F11" s="75">
+      <c r="F11" s="73">
         <f>E11+59</f>
         <v>44056</v>
       </c>
-      <c r="G11" s="115">
+      <c r="G11" s="135">
         <f t="shared" ref="G11:G22" si="4">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v>60</v>
       </c>
-      <c r="H11" s="116"/>
-      <c r="I11" s="65"/>
-      <c r="J11" s="66"/>
-      <c r="K11" s="66"/>
-      <c r="L11" s="66"/>
-      <c r="M11" s="66"/>
-      <c r="N11" s="66"/>
-      <c r="O11" s="66"/>
-      <c r="P11" s="66"/>
-      <c r="Q11" s="66"/>
-      <c r="R11" s="66"/>
-      <c r="S11" s="66"/>
-      <c r="T11" s="66"/>
-      <c r="U11" s="66"/>
-      <c r="V11" s="66"/>
-      <c r="W11" s="66"/>
-      <c r="X11" s="66"/>
-      <c r="Y11" s="46"/>
-      <c r="Z11" s="66"/>
-      <c r="AA11" s="66"/>
-      <c r="AB11" s="66"/>
-      <c r="AC11" s="66"/>
-      <c r="AD11" s="66"/>
-      <c r="AE11" s="66"/>
-      <c r="AF11" s="66"/>
-      <c r="AG11" s="66"/>
-      <c r="AH11" s="66"/>
-      <c r="AI11" s="66"/>
-      <c r="AJ11" s="66"/>
-      <c r="AK11" s="66"/>
-      <c r="AL11" s="66"/>
-      <c r="AM11" s="66"/>
-      <c r="AN11" s="66"/>
-      <c r="AO11" s="66"/>
-      <c r="AP11" s="66"/>
-      <c r="AQ11" s="66"/>
-      <c r="AR11" s="66"/>
-      <c r="AS11" s="66"/>
-      <c r="AT11" s="66"/>
-      <c r="AU11" s="66"/>
-      <c r="AV11" s="66"/>
-      <c r="AW11" s="66"/>
-      <c r="AX11" s="66"/>
-      <c r="AY11" s="66"/>
-      <c r="AZ11" s="66"/>
-      <c r="BA11" s="66"/>
-      <c r="BB11" s="66"/>
-      <c r="BC11" s="66"/>
-      <c r="BD11" s="66"/>
-      <c r="BE11" s="66"/>
-      <c r="BF11" s="66"/>
-      <c r="BG11" s="66"/>
-      <c r="BH11" s="66"/>
-      <c r="BI11" s="66"/>
-      <c r="BJ11" s="66"/>
-      <c r="BK11" s="66"/>
-      <c r="BL11" s="66"/>
-      <c r="BM11" s="66"/>
-      <c r="BN11" s="66"/>
-      <c r="BO11" s="66"/>
-      <c r="BP11" s="67"/>
-      <c r="BQ11" s="94"/>
+      <c r="H11" s="136"/>
+      <c r="I11" s="63"/>
+      <c r="J11" s="64"/>
+      <c r="K11" s="64"/>
+      <c r="L11" s="64"/>
+      <c r="M11" s="64"/>
+      <c r="N11" s="64"/>
+      <c r="O11" s="64"/>
+      <c r="P11" s="64"/>
+      <c r="Q11" s="64"/>
+      <c r="R11" s="64"/>
+      <c r="S11" s="64"/>
+      <c r="T11" s="64"/>
+      <c r="U11" s="64"/>
+      <c r="V11" s="64"/>
+      <c r="W11" s="64"/>
+      <c r="X11" s="64"/>
+      <c r="Y11" s="45"/>
+      <c r="Z11" s="64"/>
+      <c r="AA11" s="64"/>
+      <c r="AB11" s="64"/>
+      <c r="AC11" s="64"/>
+      <c r="AD11" s="64"/>
+      <c r="AE11" s="64"/>
+      <c r="AF11" s="64"/>
+      <c r="AG11" s="64"/>
+      <c r="AH11" s="64"/>
+      <c r="AI11" s="64"/>
+      <c r="AJ11" s="64"/>
+      <c r="AK11" s="64"/>
+      <c r="AL11" s="64"/>
+      <c r="AM11" s="64"/>
+      <c r="AN11" s="64"/>
+      <c r="AO11" s="64"/>
+      <c r="AP11" s="64"/>
+      <c r="AQ11" s="64"/>
+      <c r="AR11" s="64"/>
+      <c r="AS11" s="64"/>
+      <c r="AT11" s="64"/>
+      <c r="AU11" s="64"/>
+      <c r="AV11" s="64"/>
+      <c r="AW11" s="64"/>
+      <c r="AX11" s="64"/>
+      <c r="AY11" s="64"/>
+      <c r="AZ11" s="64"/>
+      <c r="BA11" s="64"/>
+      <c r="BB11" s="64"/>
+      <c r="BC11" s="64"/>
+      <c r="BD11" s="64"/>
+      <c r="BE11" s="64"/>
+      <c r="BF11" s="64"/>
+      <c r="BG11" s="64"/>
+      <c r="BH11" s="64"/>
+      <c r="BI11" s="64"/>
+      <c r="BJ11" s="64"/>
+      <c r="BK11" s="64"/>
+      <c r="BL11" s="64"/>
+      <c r="BM11" s="64"/>
+      <c r="BN11" s="64"/>
+      <c r="BO11" s="64"/>
+      <c r="BP11" s="65"/>
+      <c r="BQ11" s="91"/>
     </row>
     <row r="12" spans="1:69" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="111" t="s">
-        <v>53</v>
-      </c>
-      <c r="C12" s="112"/>
+      <c r="B12" s="128" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" s="129"/>
       <c r="D12" s="12">
-        <v>0.4</v>
-      </c>
-      <c r="E12" s="73">
-        <f>Project_Start</f>
-        <v>43997</v>
-      </c>
-      <c r="F12" s="76">
-        <f>E12+6</f>
-        <v>44003</v>
-      </c>
-      <c r="G12" s="117">
+        <v>0.2</v>
+      </c>
+      <c r="E12" s="71">
+        <v>44055</v>
+      </c>
+      <c r="F12" s="74">
+        <v>44056</v>
+      </c>
+      <c r="G12" s="137">
         <f t="shared" si="4"/>
-        <v>7</v>
-      </c>
-      <c r="H12" s="118"/>
-      <c r="I12" s="48"/>
+        <v>2</v>
+      </c>
+      <c r="H12" s="138"/>
+      <c r="I12" s="47"/>
       <c r="J12" s="33"/>
-      <c r="K12" s="143"/>
+      <c r="K12" s="142"/>
       <c r="L12" s="143"/>
       <c r="M12" s="33"/>
       <c r="N12" s="33"/>
@@ -3438,7 +3616,7 @@
       <c r="V12" s="33"/>
       <c r="W12" s="33"/>
       <c r="X12" s="33"/>
-      <c r="Y12" s="45"/>
+      <c r="Y12" s="44"/>
       <c r="Z12" s="33"/>
       <c r="AA12" s="33"/>
       <c r="AB12" s="33"/>
@@ -3482,41 +3660,39 @@
       <c r="BN12" s="33"/>
       <c r="BO12" s="33"/>
       <c r="BP12" s="33"/>
-      <c r="BQ12" s="95"/>
+      <c r="BQ12" s="92"/>
     </row>
     <row r="13" spans="1:69" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="111" t="s">
+      <c r="B13" s="128" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="112"/>
+      <c r="C13" s="129"/>
       <c r="D13" s="12">
         <v>0</v>
       </c>
-      <c r="E13" s="73">
-        <f>F12+1</f>
-        <v>44004</v>
-      </c>
-      <c r="F13" s="76">
-        <f>E13+1</f>
-        <v>44005</v>
-      </c>
-      <c r="G13" s="117">
+      <c r="E13" s="71">
+        <v>44055</v>
+      </c>
+      <c r="F13" s="74">
+        <v>44056</v>
+      </c>
+      <c r="G13" s="137">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="H13" s="118"/>
-      <c r="I13" s="47"/>
+      <c r="H13" s="138"/>
+      <c r="I13" s="46"/>
       <c r="J13" s="33"/>
       <c r="K13" s="33"/>
       <c r="L13" s="33"/>
-      <c r="M13" s="33"/>
-      <c r="N13" s="33"/>
-      <c r="O13" s="33"/>
-      <c r="P13" s="33"/>
-      <c r="Q13" s="33"/>
+      <c r="M13" s="146"/>
+      <c r="N13" s="147"/>
+      <c r="O13" s="147"/>
+      <c r="P13" s="147"/>
+      <c r="Q13" s="148"/>
       <c r="R13" s="33"/>
       <c r="S13" s="33"/>
       <c r="T13" s="33"/>
@@ -3524,7 +3700,7 @@
       <c r="V13" s="34"/>
       <c r="W13" s="33"/>
       <c r="X13" s="33"/>
-      <c r="Y13" s="45"/>
+      <c r="Y13" s="44"/>
       <c r="Z13" s="33"/>
       <c r="AA13" s="33"/>
       <c r="AB13" s="33"/>
@@ -3568,279 +3744,275 @@
       <c r="BN13" s="33"/>
       <c r="BO13" s="33"/>
       <c r="BP13" s="33"/>
-      <c r="BQ13" s="95"/>
+      <c r="BQ13" s="92"/>
     </row>
     <row r="14" spans="1:69" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="25"/>
-      <c r="B14" s="123" t="s">
+      <c r="B14" s="126" t="s">
         <v>41</v>
       </c>
-      <c r="C14" s="124"/>
-      <c r="D14" s="50">
-        <v>0</v>
-      </c>
-      <c r="E14" s="74">
-        <f>E13+1</f>
-        <v>44005</v>
-      </c>
-      <c r="F14" s="77">
-        <f>E14+7</f>
-        <v>44012</v>
-      </c>
-      <c r="G14" s="109">
+      <c r="C14" s="127"/>
+      <c r="D14" s="49">
+        <v>1</v>
+      </c>
+      <c r="E14" s="72">
+        <v>44053</v>
+      </c>
+      <c r="F14" s="75">
+        <v>44055</v>
+      </c>
+      <c r="G14" s="131">
         <f t="shared" si="4"/>
-        <v>8</v>
-      </c>
-      <c r="H14" s="110"/>
-      <c r="I14" s="51"/>
-      <c r="J14" s="52"/>
-      <c r="K14" s="52"/>
-      <c r="L14" s="52"/>
-      <c r="M14" s="52"/>
-      <c r="N14" s="52"/>
-      <c r="O14" s="52"/>
-      <c r="P14" s="52"/>
-      <c r="Q14" s="53"/>
-      <c r="R14" s="52"/>
-      <c r="S14" s="52"/>
-      <c r="T14" s="52"/>
-      <c r="U14" s="52"/>
-      <c r="V14" s="52"/>
-      <c r="W14" s="52"/>
-      <c r="X14" s="52"/>
-      <c r="Y14" s="45"/>
-      <c r="Z14" s="52"/>
-      <c r="AA14" s="52"/>
-      <c r="AB14" s="52"/>
-      <c r="AC14" s="52"/>
-      <c r="AD14" s="52"/>
-      <c r="AE14" s="52"/>
-      <c r="AF14" s="52"/>
-      <c r="AG14" s="52"/>
-      <c r="AH14" s="52"/>
-      <c r="AI14" s="52"/>
-      <c r="AJ14" s="52"/>
-      <c r="AK14" s="52"/>
-      <c r="AL14" s="52"/>
-      <c r="AM14" s="52"/>
-      <c r="AN14" s="52"/>
-      <c r="AO14" s="52"/>
-      <c r="AP14" s="52"/>
-      <c r="AQ14" s="52"/>
-      <c r="AR14" s="52"/>
-      <c r="AS14" s="52"/>
-      <c r="AT14" s="52"/>
-      <c r="AU14" s="52"/>
-      <c r="AV14" s="52"/>
-      <c r="AW14" s="52"/>
-      <c r="AX14" s="52"/>
-      <c r="AY14" s="52"/>
-      <c r="AZ14" s="52"/>
-      <c r="BA14" s="52"/>
-      <c r="BB14" s="52"/>
-      <c r="BC14" s="52"/>
-      <c r="BD14" s="52"/>
-      <c r="BE14" s="52"/>
-      <c r="BF14" s="52"/>
-      <c r="BG14" s="52"/>
-      <c r="BH14" s="52"/>
-      <c r="BI14" s="52"/>
-      <c r="BJ14" s="52"/>
-      <c r="BK14" s="52"/>
-      <c r="BL14" s="52"/>
-      <c r="BM14" s="52"/>
-      <c r="BN14" s="52"/>
-      <c r="BO14" s="52"/>
-      <c r="BP14" s="52"/>
-      <c r="BQ14" s="95"/>
+        <v>3</v>
+      </c>
+      <c r="H14" s="132"/>
+      <c r="I14" s="50"/>
+      <c r="J14" s="51"/>
+      <c r="K14" s="51"/>
+      <c r="L14" s="51"/>
+      <c r="M14" s="51"/>
+      <c r="N14" s="51"/>
+      <c r="O14" s="149"/>
+      <c r="P14" s="150"/>
+      <c r="Q14" s="151"/>
+      <c r="R14" s="152"/>
+      <c r="S14" s="51"/>
+      <c r="T14" s="51"/>
+      <c r="U14" s="51"/>
+      <c r="V14" s="51"/>
+      <c r="W14" s="51"/>
+      <c r="X14" s="51"/>
+      <c r="Y14" s="44"/>
+      <c r="Z14" s="51"/>
+      <c r="AA14" s="51"/>
+      <c r="AB14" s="51"/>
+      <c r="AC14" s="51"/>
+      <c r="AD14" s="51"/>
+      <c r="AE14" s="51"/>
+      <c r="AF14" s="51"/>
+      <c r="AG14" s="51"/>
+      <c r="AH14" s="51"/>
+      <c r="AI14" s="51"/>
+      <c r="AJ14" s="51"/>
+      <c r="AK14" s="51"/>
+      <c r="AL14" s="51"/>
+      <c r="AM14" s="51"/>
+      <c r="AN14" s="51"/>
+      <c r="AO14" s="51"/>
+      <c r="AP14" s="51"/>
+      <c r="AQ14" s="51"/>
+      <c r="AR14" s="51"/>
+      <c r="AS14" s="51"/>
+      <c r="AT14" s="51"/>
+      <c r="AU14" s="51"/>
+      <c r="AV14" s="51"/>
+      <c r="AW14" s="51"/>
+      <c r="AX14" s="51"/>
+      <c r="AY14" s="51"/>
+      <c r="AZ14" s="51"/>
+      <c r="BA14" s="51"/>
+      <c r="BB14" s="51"/>
+      <c r="BC14" s="51"/>
+      <c r="BD14" s="51"/>
+      <c r="BE14" s="51"/>
+      <c r="BF14" s="51"/>
+      <c r="BG14" s="51"/>
+      <c r="BH14" s="51"/>
+      <c r="BI14" s="51"/>
+      <c r="BJ14" s="51"/>
+      <c r="BK14" s="51"/>
+      <c r="BL14" s="51"/>
+      <c r="BM14" s="51"/>
+      <c r="BN14" s="51"/>
+      <c r="BO14" s="51"/>
+      <c r="BP14" s="51"/>
+      <c r="BQ14" s="92"/>
     </row>
     <row r="15" spans="1:69" s="3" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="100" t="s">
+      <c r="B15" s="97" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="57"/>
-      <c r="D15" s="58">
+      <c r="C15" s="55"/>
+      <c r="D15" s="56">
         <f>(D16*DATEDIF(E16,F16,"D")+D17*DATEDIF(E17,F17,"D")+D18*DATEDIF(E18,F18,"D")+D19*DATEDIF(E19,F19,"D")+D20*DATEDIF(E20,F20,"D")+D21*DATEDIF(E21,F21,"D")+D22*DATEDIF(E22,F22,"D"))/(DATEDIF(E16,F16,"D")+DATEDIF(E17,F17,"D")+DATEDIF(E18,F18,"D")+DATEDIF(E19,F19,"D")+DATEDIF(E20,F20,"D")+DATEDIF(E21,F21,"D")+DATEDIF(E22,F22,"D"))</f>
-        <v>9.7341772151898737E-2</v>
-      </c>
-      <c r="E15" s="59"/>
-      <c r="F15" s="60"/>
-      <c r="G15" s="108">
+        <v>0.5066037735849056</v>
+      </c>
+      <c r="E15" s="57"/>
+      <c r="F15" s="58"/>
+      <c r="G15" s="130">
         <f ca="1">DATEDIF(E16,NOW(), "D")/DATEDIF(E16,BQ7,"d")</f>
-        <v>0.22033898305084745</v>
-      </c>
-      <c r="H15" s="108"/>
-      <c r="I15" s="61"/>
-      <c r="J15" s="61"/>
-      <c r="K15" s="61"/>
-      <c r="L15" s="61"/>
-      <c r="M15" s="61"/>
-      <c r="N15" s="61"/>
-      <c r="O15" s="61"/>
-      <c r="P15" s="61"/>
-      <c r="Q15" s="61"/>
-      <c r="R15" s="61"/>
-      <c r="S15" s="61"/>
-      <c r="T15" s="61"/>
-      <c r="U15" s="61"/>
-      <c r="V15" s="61"/>
-      <c r="W15" s="61"/>
-      <c r="X15" s="61"/>
-      <c r="Y15" s="81"/>
-      <c r="Z15" s="61"/>
-      <c r="AA15" s="61"/>
-      <c r="AB15" s="61"/>
-      <c r="AC15" s="61"/>
-      <c r="AD15" s="61"/>
-      <c r="AE15" s="61"/>
-      <c r="AF15" s="61"/>
-      <c r="AG15" s="61"/>
-      <c r="AH15" s="61"/>
-      <c r="AI15" s="61"/>
-      <c r="AJ15" s="61"/>
-      <c r="AK15" s="61"/>
-      <c r="AL15" s="61"/>
-      <c r="AM15" s="61"/>
-      <c r="AN15" s="61"/>
-      <c r="AO15" s="61"/>
-      <c r="AP15" s="61"/>
-      <c r="AQ15" s="61"/>
-      <c r="AR15" s="61"/>
-      <c r="AS15" s="61"/>
-      <c r="AT15" s="61"/>
-      <c r="AU15" s="61"/>
-      <c r="AV15" s="61"/>
-      <c r="AW15" s="61"/>
-      <c r="AX15" s="61"/>
-      <c r="AY15" s="61"/>
-      <c r="AZ15" s="61"/>
-      <c r="BA15" s="61"/>
-      <c r="BB15" s="61"/>
-      <c r="BC15" s="61"/>
-      <c r="BD15" s="61"/>
-      <c r="BE15" s="61"/>
-      <c r="BF15" s="61"/>
-      <c r="BG15" s="61"/>
-      <c r="BH15" s="61"/>
-      <c r="BI15" s="61"/>
-      <c r="BJ15" s="61"/>
-      <c r="BK15" s="61"/>
-      <c r="BL15" s="61"/>
-      <c r="BM15" s="61"/>
-      <c r="BN15" s="61"/>
-      <c r="BO15" s="61"/>
-      <c r="BP15" s="62"/>
-      <c r="BQ15" s="96"/>
+        <v>0.96610169491525422</v>
+      </c>
+      <c r="H15" s="130"/>
+      <c r="I15" s="59"/>
+      <c r="J15" s="59"/>
+      <c r="K15" s="59"/>
+      <c r="L15" s="59"/>
+      <c r="M15" s="59"/>
+      <c r="N15" s="59"/>
+      <c r="O15" s="59"/>
+      <c r="P15" s="59"/>
+      <c r="Q15" s="59"/>
+      <c r="R15" s="154"/>
+      <c r="S15" s="154"/>
+      <c r="T15" s="59"/>
+      <c r="U15" s="59"/>
+      <c r="V15" s="59"/>
+      <c r="W15" s="59"/>
+      <c r="X15" s="59"/>
+      <c r="Y15" s="79"/>
+      <c r="Z15" s="59"/>
+      <c r="AA15" s="59"/>
+      <c r="AB15" s="59"/>
+      <c r="AC15" s="59"/>
+      <c r="AD15" s="59"/>
+      <c r="AE15" s="59"/>
+      <c r="AF15" s="59"/>
+      <c r="AG15" s="59"/>
+      <c r="AH15" s="59"/>
+      <c r="AI15" s="59"/>
+      <c r="AJ15" s="59"/>
+      <c r="AK15" s="59"/>
+      <c r="AL15" s="59"/>
+      <c r="AM15" s="59"/>
+      <c r="AN15" s="59"/>
+      <c r="AO15" s="59"/>
+      <c r="AP15" s="59"/>
+      <c r="AQ15" s="59"/>
+      <c r="AR15" s="59"/>
+      <c r="AS15" s="59"/>
+      <c r="AT15" s="59"/>
+      <c r="AU15" s="59"/>
+      <c r="AV15" s="59"/>
+      <c r="AW15" s="59"/>
+      <c r="AX15" s="59"/>
+      <c r="AY15" s="59"/>
+      <c r="AZ15" s="59"/>
+      <c r="BA15" s="59"/>
+      <c r="BB15" s="59"/>
+      <c r="BC15" s="59"/>
+      <c r="BD15" s="59"/>
+      <c r="BE15" s="59"/>
+      <c r="BF15" s="59"/>
+      <c r="BG15" s="59"/>
+      <c r="BH15" s="59"/>
+      <c r="BI15" s="59"/>
+      <c r="BJ15" s="59"/>
+      <c r="BK15" s="59"/>
+      <c r="BL15" s="59"/>
+      <c r="BM15" s="59"/>
+      <c r="BN15" s="59"/>
+      <c r="BO15" s="59"/>
+      <c r="BP15" s="60"/>
+      <c r="BQ15" s="93"/>
     </row>
     <row r="16" spans="1:69" s="3" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="26"/>
-      <c r="B16" s="121" t="s">
+      <c r="B16" s="124" t="s">
         <v>49</v>
       </c>
-      <c r="C16" s="122"/>
-      <c r="D16" s="54">
+      <c r="C16" s="125"/>
+      <c r="D16" s="52">
         <v>1</v>
       </c>
-      <c r="E16" s="78">
+      <c r="E16" s="76">
         <v>43998</v>
       </c>
-      <c r="F16" s="78">
+      <c r="F16" s="76">
         <f>E16+1</f>
         <v>43999</v>
       </c>
-      <c r="G16" s="133">
+      <c r="G16" s="116">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="H16" s="134"/>
-      <c r="I16" s="55"/>
-      <c r="J16" s="56"/>
-      <c r="K16" s="56"/>
-      <c r="L16" s="56"/>
-      <c r="M16" s="56"/>
-      <c r="N16" s="56"/>
-      <c r="O16" s="56"/>
-      <c r="P16" s="56"/>
-      <c r="Q16" s="56"/>
-      <c r="R16" s="56"/>
-      <c r="S16" s="56"/>
-      <c r="T16" s="56"/>
-      <c r="U16" s="56"/>
-      <c r="V16" s="56"/>
-      <c r="W16" s="56"/>
-      <c r="X16" s="56"/>
-      <c r="Y16" s="45"/>
-      <c r="Z16" s="56"/>
-      <c r="AA16" s="56"/>
-      <c r="AB16" s="56"/>
-      <c r="AC16" s="56"/>
-      <c r="AD16" s="56"/>
-      <c r="AE16" s="56"/>
-      <c r="AF16" s="56"/>
-      <c r="AG16" s="56"/>
-      <c r="AH16" s="56"/>
-      <c r="AI16" s="56"/>
-      <c r="AJ16" s="56"/>
-      <c r="AK16" s="56"/>
-      <c r="AL16" s="56"/>
-      <c r="AM16" s="56"/>
-      <c r="AN16" s="56"/>
-      <c r="AO16" s="56"/>
-      <c r="AP16" s="56"/>
-      <c r="AQ16" s="56"/>
-      <c r="AR16" s="56"/>
-      <c r="AS16" s="56"/>
-      <c r="AT16" s="56"/>
-      <c r="AU16" s="56"/>
-      <c r="AV16" s="56"/>
-      <c r="AW16" s="56"/>
-      <c r="AX16" s="56"/>
-      <c r="AY16" s="56"/>
-      <c r="AZ16" s="56"/>
-      <c r="BA16" s="56"/>
-      <c r="BB16" s="56"/>
-      <c r="BC16" s="56"/>
-      <c r="BD16" s="56"/>
-      <c r="BE16" s="56"/>
-      <c r="BF16" s="56"/>
-      <c r="BG16" s="56"/>
-      <c r="BH16" s="56"/>
-      <c r="BI16" s="56"/>
-      <c r="BJ16" s="56"/>
-      <c r="BK16" s="56"/>
-      <c r="BL16" s="56"/>
-      <c r="BM16" s="56"/>
-      <c r="BN16" s="56"/>
-      <c r="BO16" s="56"/>
-      <c r="BP16" s="56"/>
-      <c r="BQ16" s="95"/>
+      <c r="H16" s="117"/>
+      <c r="I16" s="53"/>
+      <c r="J16" s="54"/>
+      <c r="K16" s="54"/>
+      <c r="L16" s="54"/>
+      <c r="M16" s="54"/>
+      <c r="N16" s="54"/>
+      <c r="O16" s="54"/>
+      <c r="P16" s="54"/>
+      <c r="Q16" s="153"/>
+      <c r="R16" s="155"/>
+      <c r="S16" s="157"/>
+      <c r="T16" s="158"/>
+      <c r="U16" s="159"/>
+      <c r="V16" s="159"/>
+      <c r="W16" s="159"/>
+      <c r="X16" s="159"/>
+      <c r="Y16" s="44"/>
+      <c r="Z16" s="159"/>
+      <c r="AA16" s="159"/>
+      <c r="AB16" s="159"/>
+      <c r="AC16" s="159"/>
+      <c r="AD16" s="159"/>
+      <c r="AE16" s="159"/>
+      <c r="AF16" s="159"/>
+      <c r="AG16" s="159"/>
+      <c r="AH16" s="159"/>
+      <c r="AI16" s="159"/>
+      <c r="AJ16" s="159"/>
+      <c r="AK16" s="159"/>
+      <c r="AL16" s="159"/>
+      <c r="AM16" s="159"/>
+      <c r="AN16" s="159"/>
+      <c r="AO16" s="159"/>
+      <c r="AP16" s="159"/>
+      <c r="AQ16" s="54"/>
+      <c r="AR16" s="54"/>
+      <c r="AS16" s="54"/>
+      <c r="AT16" s="54"/>
+      <c r="AU16" s="54"/>
+      <c r="AV16" s="54"/>
+      <c r="AW16" s="54"/>
+      <c r="AX16" s="54"/>
+      <c r="AY16" s="54"/>
+      <c r="AZ16" s="54"/>
+      <c r="BA16" s="54"/>
+      <c r="BB16" s="54"/>
+      <c r="BC16" s="54"/>
+      <c r="BD16" s="54"/>
+      <c r="BE16" s="54"/>
+      <c r="BF16" s="54"/>
+      <c r="BG16" s="54"/>
+      <c r="BH16" s="54"/>
+      <c r="BI16" s="54"/>
+      <c r="BJ16" s="54"/>
+      <c r="BK16" s="54"/>
+      <c r="BL16" s="54"/>
+      <c r="BM16" s="54"/>
+      <c r="BN16" s="54"/>
+      <c r="BO16" s="54"/>
+      <c r="BP16" s="54"/>
+      <c r="BQ16" s="92"/>
     </row>
     <row r="17" spans="1:69" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="26"/>
-      <c r="B17" s="119" t="s">
+      <c r="B17" s="122" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="120"/>
+      <c r="C17" s="123"/>
       <c r="D17" s="13">
-        <v>0.2</v>
-      </c>
-      <c r="E17" s="79">
-        <f>F14-12</f>
-        <v>44000</v>
-      </c>
-      <c r="F17" s="79">
-        <f>E17+31</f>
-        <v>44031</v>
-      </c>
-      <c r="G17" s="125">
+        <v>0.95</v>
+      </c>
+      <c r="E17" s="77">
+        <v>44033</v>
+      </c>
+      <c r="F17" s="77">
+        <v>44056</v>
+      </c>
+      <c r="G17" s="111">
         <f t="shared" si="4"/>
-        <v>32</v>
-      </c>
-      <c r="H17" s="126"/>
-      <c r="I17" s="49"/>
+        <v>24</v>
+      </c>
+      <c r="H17" s="112"/>
+      <c r="I17" s="48"/>
       <c r="J17" s="35"/>
       <c r="K17" s="35"/>
       <c r="L17" s="35"/>
@@ -3849,34 +4021,34 @@
       <c r="O17" s="35"/>
       <c r="P17" s="35"/>
       <c r="Q17" s="35"/>
-      <c r="R17" s="35"/>
-      <c r="S17" s="35"/>
-      <c r="T17" s="35"/>
-      <c r="U17" s="35"/>
-      <c r="V17" s="35"/>
-      <c r="W17" s="35"/>
-      <c r="X17" s="35"/>
-      <c r="Y17" s="45"/>
-      <c r="Z17" s="35"/>
-      <c r="AA17" s="35"/>
-      <c r="AB17" s="35"/>
-      <c r="AC17" s="35"/>
-      <c r="AD17" s="35"/>
-      <c r="AE17" s="35"/>
-      <c r="AF17" s="35"/>
-      <c r="AG17" s="35"/>
-      <c r="AH17" s="35"/>
-      <c r="AI17" s="35"/>
-      <c r="AJ17" s="35"/>
-      <c r="AK17" s="35"/>
-      <c r="AL17" s="35"/>
-      <c r="AM17" s="35"/>
-      <c r="AN17" s="35"/>
-      <c r="AO17" s="35"/>
-      <c r="AP17" s="35"/>
-      <c r="AQ17" s="35"/>
-      <c r="AR17" s="35"/>
-      <c r="AS17" s="35"/>
+      <c r="R17" s="153"/>
+      <c r="S17" s="155"/>
+      <c r="T17" s="160"/>
+      <c r="U17" s="160"/>
+      <c r="V17" s="160"/>
+      <c r="W17" s="160"/>
+      <c r="X17" s="160"/>
+      <c r="Y17" s="161"/>
+      <c r="Z17" s="160"/>
+      <c r="AA17" s="160"/>
+      <c r="AB17" s="160"/>
+      <c r="AC17" s="160"/>
+      <c r="AD17" s="160"/>
+      <c r="AE17" s="160"/>
+      <c r="AF17" s="160"/>
+      <c r="AG17" s="160"/>
+      <c r="AH17" s="162"/>
+      <c r="AI17" s="162"/>
+      <c r="AJ17" s="162"/>
+      <c r="AK17" s="162"/>
+      <c r="AL17" s="162"/>
+      <c r="AM17" s="162"/>
+      <c r="AN17" s="162"/>
+      <c r="AO17" s="162"/>
+      <c r="AP17" s="157"/>
+      <c r="AQ17" s="163"/>
+      <c r="AR17" s="164"/>
+      <c r="AS17" s="164"/>
       <c r="AT17" s="35"/>
       <c r="AU17" s="35"/>
       <c r="AV17" s="35"/>
@@ -3900,31 +4072,31 @@
       <c r="BN17" s="35"/>
       <c r="BO17" s="35"/>
       <c r="BP17" s="35"/>
-      <c r="BQ17" s="95"/>
+      <c r="BQ17" s="92"/>
     </row>
     <row r="18" spans="1:69" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="25"/>
-      <c r="B18" s="119" t="s">
+      <c r="B18" s="122" t="s">
         <v>45</v>
       </c>
-      <c r="C18" s="120"/>
+      <c r="C18" s="123"/>
       <c r="D18" s="13">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="E18" s="79">
+        <v>0.5</v>
+      </c>
+      <c r="E18" s="77">
         <f>F17-7</f>
-        <v>44024</v>
-      </c>
-      <c r="F18" s="79">
+        <v>44049</v>
+      </c>
+      <c r="F18" s="77">
         <f>E18+7</f>
-        <v>44031</v>
-      </c>
-      <c r="G18" s="125">
+        <v>44056</v>
+      </c>
+      <c r="G18" s="111">
         <f t="shared" si="4"/>
         <v>8</v>
       </c>
-      <c r="H18" s="126"/>
-      <c r="I18" s="49"/>
+      <c r="H18" s="112"/>
+      <c r="I18" s="48"/>
       <c r="J18" s="35"/>
       <c r="K18" s="35"/>
       <c r="L18" s="35"/>
@@ -3934,38 +4106,38 @@
       <c r="P18" s="35"/>
       <c r="Q18" s="35"/>
       <c r="R18" s="35"/>
-      <c r="S18" s="35"/>
-      <c r="T18" s="35"/>
-      <c r="U18" s="35"/>
-      <c r="V18" s="35"/>
-      <c r="W18" s="35"/>
-      <c r="X18" s="35"/>
-      <c r="Y18" s="46"/>
-      <c r="Z18" s="35"/>
-      <c r="AA18" s="35"/>
-      <c r="AB18" s="35"/>
-      <c r="AC18" s="35"/>
-      <c r="AD18" s="35"/>
-      <c r="AE18" s="35"/>
-      <c r="AF18" s="35"/>
-      <c r="AG18" s="35"/>
-      <c r="AH18" s="35"/>
-      <c r="AI18" s="35"/>
-      <c r="AJ18" s="35"/>
-      <c r="AK18" s="35"/>
-      <c r="AL18" s="35"/>
-      <c r="AM18" s="35"/>
-      <c r="AN18" s="35"/>
-      <c r="AO18" s="35"/>
-      <c r="AP18" s="35"/>
-      <c r="AQ18" s="35"/>
-      <c r="AR18" s="35"/>
-      <c r="AS18" s="35"/>
-      <c r="AT18" s="35"/>
-      <c r="AU18" s="35"/>
-      <c r="AV18" s="35"/>
-      <c r="AW18" s="35"/>
-      <c r="AX18" s="35"/>
+      <c r="S18" s="54"/>
+      <c r="T18" s="54"/>
+      <c r="U18" s="54"/>
+      <c r="V18" s="54"/>
+      <c r="W18" s="54"/>
+      <c r="X18" s="54"/>
+      <c r="Y18" s="45"/>
+      <c r="Z18" s="54"/>
+      <c r="AA18" s="54"/>
+      <c r="AB18" s="54"/>
+      <c r="AC18" s="54"/>
+      <c r="AD18" s="54"/>
+      <c r="AE18" s="54"/>
+      <c r="AF18" s="54"/>
+      <c r="AG18" s="153"/>
+      <c r="AH18" s="155"/>
+      <c r="AI18" s="160"/>
+      <c r="AJ18" s="160"/>
+      <c r="AK18" s="160"/>
+      <c r="AL18" s="160"/>
+      <c r="AM18" s="160"/>
+      <c r="AN18" s="160"/>
+      <c r="AO18" s="162"/>
+      <c r="AP18" s="162"/>
+      <c r="AQ18" s="162"/>
+      <c r="AR18" s="162"/>
+      <c r="AS18" s="157"/>
+      <c r="AT18" s="163"/>
+      <c r="AU18" s="164"/>
+      <c r="AV18" s="164"/>
+      <c r="AW18" s="164"/>
+      <c r="AX18" s="164"/>
       <c r="AY18" s="35"/>
       <c r="AZ18" s="35"/>
       <c r="BA18" s="35"/>
@@ -3984,31 +4156,31 @@
       <c r="BN18" s="35"/>
       <c r="BO18" s="35"/>
       <c r="BP18" s="35"/>
-      <c r="BQ18" s="95"/>
+      <c r="BQ18" s="92"/>
     </row>
     <row r="19" spans="1:69" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="25"/>
-      <c r="B19" s="119" t="s">
+      <c r="B19" s="122" t="s">
         <v>44</v>
       </c>
-      <c r="C19" s="120"/>
+      <c r="C19" s="123"/>
       <c r="D19" s="13">
         <v>0</v>
       </c>
-      <c r="E19" s="79">
+      <c r="E19" s="77">
         <f>F17-7</f>
-        <v>44024</v>
-      </c>
-      <c r="F19" s="79">
+        <v>44049</v>
+      </c>
+      <c r="F19" s="77">
         <f>E19+10</f>
-        <v>44034</v>
-      </c>
-      <c r="G19" s="125">
+        <v>44059</v>
+      </c>
+      <c r="G19" s="111">
         <f t="shared" si="4"/>
         <v>11</v>
       </c>
-      <c r="H19" s="126"/>
-      <c r="I19" s="49"/>
+      <c r="H19" s="112"/>
+      <c r="I19" s="48"/>
       <c r="J19" s="35"/>
       <c r="K19" s="35"/>
       <c r="L19" s="35"/>
@@ -4024,7 +4196,7 @@
       <c r="V19" s="36"/>
       <c r="W19" s="35"/>
       <c r="X19" s="35"/>
-      <c r="Y19" s="45"/>
+      <c r="Y19" s="44"/>
       <c r="Z19" s="35"/>
       <c r="AA19" s="35"/>
       <c r="AB19" s="35"/>
@@ -4033,25 +4205,25 @@
       <c r="AE19" s="35"/>
       <c r="AF19" s="35"/>
       <c r="AG19" s="35"/>
-      <c r="AH19" s="35"/>
-      <c r="AI19" s="35"/>
-      <c r="AJ19" s="35"/>
-      <c r="AK19" s="35"/>
-      <c r="AL19" s="35"/>
-      <c r="AM19" s="35"/>
-      <c r="AN19" s="35"/>
-      <c r="AO19" s="35"/>
-      <c r="AP19" s="35"/>
-      <c r="AQ19" s="35"/>
-      <c r="AR19" s="35"/>
-      <c r="AS19" s="35"/>
-      <c r="AT19" s="35"/>
-      <c r="AU19" s="35"/>
-      <c r="AV19" s="35"/>
-      <c r="AW19" s="35"/>
-      <c r="AX19" s="35"/>
-      <c r="AY19" s="35"/>
-      <c r="AZ19" s="35"/>
+      <c r="AH19" s="54"/>
+      <c r="AI19" s="54"/>
+      <c r="AJ19" s="54"/>
+      <c r="AK19" s="54"/>
+      <c r="AL19" s="54"/>
+      <c r="AM19" s="54"/>
+      <c r="AN19" s="153"/>
+      <c r="AO19" s="155"/>
+      <c r="AP19" s="160"/>
+      <c r="AQ19" s="160"/>
+      <c r="AR19" s="160"/>
+      <c r="AS19" s="160"/>
+      <c r="AT19" s="160"/>
+      <c r="AU19" s="160"/>
+      <c r="AV19" s="160"/>
+      <c r="AW19" s="162"/>
+      <c r="AX19" s="157"/>
+      <c r="AY19" s="163"/>
+      <c r="AZ19" s="164"/>
       <c r="BA19" s="35"/>
       <c r="BB19" s="35"/>
       <c r="BC19" s="35"/>
@@ -4068,31 +4240,31 @@
       <c r="BN19" s="35"/>
       <c r="BO19" s="35"/>
       <c r="BP19" s="35"/>
-      <c r="BQ19" s="95"/>
+      <c r="BQ19" s="92"/>
     </row>
     <row r="20" spans="1:69" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="25"/>
-      <c r="B20" s="119" t="s">
+      <c r="B20" s="122" t="s">
         <v>48</v>
       </c>
-      <c r="C20" s="120"/>
+      <c r="C20" s="123"/>
       <c r="D20" s="13">
         <v>0</v>
       </c>
-      <c r="E20" s="79">
+      <c r="E20" s="77">
         <f>F19-3</f>
-        <v>44031</v>
-      </c>
-      <c r="F20" s="79">
+        <v>44056</v>
+      </c>
+      <c r="F20" s="77">
         <f>E20+10</f>
-        <v>44041</v>
-      </c>
-      <c r="G20" s="125">
+        <v>44066</v>
+      </c>
+      <c r="G20" s="111">
         <f t="shared" si="4"/>
         <v>11</v>
       </c>
-      <c r="H20" s="126"/>
-      <c r="I20" s="49"/>
+      <c r="H20" s="112"/>
+      <c r="I20" s="48"/>
       <c r="J20" s="35"/>
       <c r="K20" s="35"/>
       <c r="L20" s="35"/>
@@ -4108,7 +4280,7 @@
       <c r="V20" s="35"/>
       <c r="W20" s="35"/>
       <c r="X20" s="35"/>
-      <c r="Y20" s="45"/>
+      <c r="Y20" s="44"/>
       <c r="Z20" s="35"/>
       <c r="AA20" s="35"/>
       <c r="AB20" s="35"/>
@@ -4123,23 +4295,23 @@
       <c r="AK20" s="35"/>
       <c r="AL20" s="35"/>
       <c r="AM20" s="35"/>
-      <c r="AN20" s="35"/>
-      <c r="AO20" s="35"/>
-      <c r="AP20" s="35"/>
-      <c r="AQ20" s="35"/>
-      <c r="AR20" s="35"/>
-      <c r="AS20" s="35"/>
-      <c r="AT20" s="35"/>
-      <c r="AU20" s="35"/>
-      <c r="AV20" s="35"/>
-      <c r="AW20" s="35"/>
-      <c r="AX20" s="35"/>
-      <c r="AY20" s="35"/>
-      <c r="AZ20" s="35"/>
-      <c r="BA20" s="35"/>
-      <c r="BB20" s="35"/>
-      <c r="BC20" s="35"/>
-      <c r="BD20" s="35"/>
+      <c r="AN20" s="164"/>
+      <c r="AO20" s="159"/>
+      <c r="AP20" s="159"/>
+      <c r="AQ20" s="54"/>
+      <c r="AR20" s="54"/>
+      <c r="AS20" s="54"/>
+      <c r="AT20" s="54"/>
+      <c r="AU20" s="54"/>
+      <c r="AV20" s="153"/>
+      <c r="AW20" s="155"/>
+      <c r="AX20" s="160"/>
+      <c r="AY20" s="162"/>
+      <c r="AZ20" s="157"/>
+      <c r="BA20" s="163"/>
+      <c r="BB20" s="164"/>
+      <c r="BC20" s="164"/>
+      <c r="BD20" s="164"/>
       <c r="BE20" s="35"/>
       <c r="BF20" s="35"/>
       <c r="BG20" s="35"/>
@@ -4152,31 +4324,29 @@
       <c r="BN20" s="35"/>
       <c r="BO20" s="35"/>
       <c r="BP20" s="35"/>
-      <c r="BQ20" s="95"/>
+      <c r="BQ20" s="92"/>
     </row>
     <row r="21" spans="1:69" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="25"/>
-      <c r="B21" s="119" t="s">
+      <c r="B21" s="122" t="s">
         <v>47</v>
       </c>
-      <c r="C21" s="120"/>
+      <c r="C21" s="123"/>
       <c r="D21" s="13">
-        <v>0</v>
-      </c>
-      <c r="E21" s="79">
-        <f>F19</f>
-        <v>44034</v>
-      </c>
-      <c r="F21" s="79">
-        <f>E21+10</f>
-        <v>44044</v>
-      </c>
-      <c r="G21" s="125">
+        <v>0.5</v>
+      </c>
+      <c r="E21" s="140">
+        <v>44055</v>
+      </c>
+      <c r="F21" s="141">
+        <v>44056</v>
+      </c>
+      <c r="G21" s="111">
         <f t="shared" si="4"/>
-        <v>11</v>
-      </c>
-      <c r="H21" s="126"/>
-      <c r="I21" s="49"/>
+        <v>2</v>
+      </c>
+      <c r="H21" s="112"/>
+      <c r="I21" s="48"/>
       <c r="J21" s="35"/>
       <c r="K21" s="35"/>
       <c r="L21" s="35"/>
@@ -4192,7 +4362,7 @@
       <c r="V21" s="35"/>
       <c r="W21" s="35"/>
       <c r="X21" s="35"/>
-      <c r="Y21" s="45"/>
+      <c r="Y21" s="44"/>
       <c r="Z21" s="35"/>
       <c r="AA21" s="35"/>
       <c r="AB21" s="35"/>
@@ -4206,28 +4376,28 @@
       <c r="AJ21" s="35"/>
       <c r="AK21" s="35"/>
       <c r="AL21" s="35"/>
-      <c r="AM21" s="35"/>
-      <c r="AN21" s="35"/>
-      <c r="AO21" s="35"/>
-      <c r="AP21" s="35"/>
-      <c r="AQ21" s="35"/>
+      <c r="AM21" s="166"/>
+      <c r="AN21" s="155"/>
+      <c r="AO21" s="160"/>
+      <c r="AP21" s="156"/>
+      <c r="AQ21" s="48"/>
       <c r="AR21" s="35"/>
       <c r="AS21" s="35"/>
       <c r="AT21" s="35"/>
       <c r="AU21" s="35"/>
       <c r="AV21" s="35"/>
-      <c r="AW21" s="35"/>
-      <c r="AX21" s="35"/>
-      <c r="AY21" s="35"/>
-      <c r="AZ21" s="35"/>
-      <c r="BA21" s="35"/>
-      <c r="BB21" s="35"/>
-      <c r="BC21" s="35"/>
-      <c r="BD21" s="35"/>
-      <c r="BE21" s="35"/>
-      <c r="BF21" s="35"/>
-      <c r="BG21" s="35"/>
-      <c r="BH21" s="35"/>
+      <c r="AW21" s="54"/>
+      <c r="AX21" s="153"/>
+      <c r="AY21" s="155"/>
+      <c r="AZ21" s="160"/>
+      <c r="BA21" s="160"/>
+      <c r="BB21" s="160"/>
+      <c r="BC21" s="160"/>
+      <c r="BD21" s="157"/>
+      <c r="BE21" s="163"/>
+      <c r="BF21" s="164"/>
+      <c r="BG21" s="164"/>
+      <c r="BH21" s="164"/>
       <c r="BI21" s="35"/>
       <c r="BJ21" s="35"/>
       <c r="BK21" s="35"/>
@@ -4236,91 +4406,89 @@
       <c r="BN21" s="35"/>
       <c r="BO21" s="35"/>
       <c r="BP21" s="35"/>
-      <c r="BQ21" s="95"/>
+      <c r="BQ21" s="92"/>
     </row>
     <row r="22" spans="1:69" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="25"/>
-      <c r="B22" s="137" t="s">
+      <c r="B22" s="120" t="s">
         <v>46</v>
       </c>
-      <c r="C22" s="138"/>
-      <c r="D22" s="85">
+      <c r="C22" s="121"/>
+      <c r="D22" s="83">
         <v>0</v>
       </c>
-      <c r="E22" s="86">
-        <f>F21-7</f>
-        <v>44037</v>
-      </c>
-      <c r="F22" s="86">
-        <f>E22+10</f>
-        <v>44047</v>
-      </c>
-      <c r="G22" s="127">
+      <c r="E22" s="140">
+        <v>44055</v>
+      </c>
+      <c r="F22" s="141">
+        <v>44056</v>
+      </c>
+      <c r="G22" s="113">
         <f t="shared" si="4"/>
-        <v>11</v>
-      </c>
-      <c r="H22" s="128"/>
-      <c r="I22" s="87"/>
-      <c r="J22" s="88"/>
-      <c r="K22" s="88"/>
-      <c r="L22" s="88"/>
-      <c r="M22" s="88"/>
-      <c r="N22" s="88"/>
-      <c r="O22" s="88"/>
-      <c r="P22" s="88"/>
-      <c r="Q22" s="88"/>
-      <c r="R22" s="88"/>
-      <c r="S22" s="88"/>
-      <c r="T22" s="88"/>
-      <c r="U22" s="88"/>
-      <c r="V22" s="88"/>
-      <c r="W22" s="88"/>
-      <c r="X22" s="88"/>
-      <c r="Y22" s="89"/>
-      <c r="Z22" s="88"/>
-      <c r="AA22" s="88"/>
-      <c r="AB22" s="88"/>
-      <c r="AC22" s="88"/>
-      <c r="AD22" s="88"/>
-      <c r="AE22" s="88"/>
-      <c r="AF22" s="88"/>
-      <c r="AG22" s="88"/>
-      <c r="AH22" s="88"/>
-      <c r="AI22" s="88"/>
-      <c r="AJ22" s="88"/>
-      <c r="AK22" s="88"/>
-      <c r="AL22" s="88"/>
-      <c r="AM22" s="88"/>
-      <c r="AN22" s="88"/>
-      <c r="AO22" s="88"/>
-      <c r="AP22" s="88"/>
-      <c r="AQ22" s="88"/>
-      <c r="AR22" s="88"/>
-      <c r="AS22" s="88"/>
-      <c r="AT22" s="88"/>
-      <c r="AU22" s="88"/>
-      <c r="AV22" s="88"/>
-      <c r="AW22" s="88"/>
-      <c r="AX22" s="88"/>
-      <c r="AY22" s="88"/>
-      <c r="AZ22" s="88"/>
-      <c r="BA22" s="88"/>
-      <c r="BB22" s="88"/>
-      <c r="BC22" s="88"/>
-      <c r="BD22" s="88"/>
-      <c r="BE22" s="88"/>
-      <c r="BF22" s="88"/>
-      <c r="BG22" s="88"/>
-      <c r="BH22" s="88"/>
-      <c r="BI22" s="88"/>
-      <c r="BJ22" s="88"/>
-      <c r="BK22" s="88"/>
-      <c r="BL22" s="88"/>
-      <c r="BM22" s="88"/>
-      <c r="BN22" s="88"/>
-      <c r="BO22" s="88"/>
-      <c r="BP22" s="88"/>
-      <c r="BQ22" s="97"/>
+        <v>2</v>
+      </c>
+      <c r="H22" s="114"/>
+      <c r="I22" s="84"/>
+      <c r="J22" s="85"/>
+      <c r="K22" s="85"/>
+      <c r="L22" s="85"/>
+      <c r="M22" s="85"/>
+      <c r="N22" s="85"/>
+      <c r="O22" s="85"/>
+      <c r="P22" s="85"/>
+      <c r="Q22" s="85"/>
+      <c r="R22" s="85"/>
+      <c r="S22" s="85"/>
+      <c r="T22" s="85"/>
+      <c r="U22" s="85"/>
+      <c r="V22" s="85"/>
+      <c r="W22" s="85"/>
+      <c r="X22" s="85"/>
+      <c r="Y22" s="86"/>
+      <c r="Z22" s="85"/>
+      <c r="AA22" s="85"/>
+      <c r="AB22" s="85"/>
+      <c r="AC22" s="85"/>
+      <c r="AD22" s="85"/>
+      <c r="AE22" s="85"/>
+      <c r="AF22" s="85"/>
+      <c r="AG22" s="85"/>
+      <c r="AH22" s="85"/>
+      <c r="AI22" s="85"/>
+      <c r="AJ22" s="85"/>
+      <c r="AK22" s="85"/>
+      <c r="AL22" s="85"/>
+      <c r="AM22" s="85"/>
+      <c r="AN22" s="165"/>
+      <c r="AO22" s="165"/>
+      <c r="AP22" s="165"/>
+      <c r="AQ22" s="85"/>
+      <c r="AR22" s="85"/>
+      <c r="AS22" s="85"/>
+      <c r="AT22" s="85"/>
+      <c r="AU22" s="85"/>
+      <c r="AV22" s="85"/>
+      <c r="AW22" s="85"/>
+      <c r="AX22" s="85"/>
+      <c r="AY22" s="165"/>
+      <c r="AZ22" s="165"/>
+      <c r="BA22" s="165"/>
+      <c r="BB22" s="165"/>
+      <c r="BC22" s="167"/>
+      <c r="BD22" s="155"/>
+      <c r="BE22" s="160"/>
+      <c r="BF22" s="160"/>
+      <c r="BG22" s="160"/>
+      <c r="BH22" s="156"/>
+      <c r="BI22" s="84"/>
+      <c r="BJ22" s="85"/>
+      <c r="BK22" s="85"/>
+      <c r="BL22" s="85"/>
+      <c r="BM22" s="85"/>
+      <c r="BN22" s="85"/>
+      <c r="BO22" s="85"/>
+      <c r="BP22" s="85"/>
+      <c r="BQ22" s="94"/>
     </row>
     <row r="23" spans="1:69" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="G23" s="6"/>
@@ -4334,14 +4502,18 @@
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="BM6:BQ6"/>
-    <mergeCell ref="G5:H6"/>
-    <mergeCell ref="I6:O6"/>
-    <mergeCell ref="P6:V6"/>
-    <mergeCell ref="W6:AC6"/>
-    <mergeCell ref="AD6:AJ6"/>
-    <mergeCell ref="AK6:AQ6"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B13:C13"/>
     <mergeCell ref="G21:H21"/>
     <mergeCell ref="G22:H22"/>
     <mergeCell ref="AR6:AX6"/>
@@ -4358,18 +4530,14 @@
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="BM6:BQ6"/>
+    <mergeCell ref="G5:H6"/>
+    <mergeCell ref="I6:O6"/>
+    <mergeCell ref="P6:V6"/>
+    <mergeCell ref="W6:AC6"/>
+    <mergeCell ref="AD6:AJ6"/>
+    <mergeCell ref="AK6:AQ6"/>
   </mergeCells>
   <conditionalFormatting sqref="AF10:AF11 BH10:BH11 D9:D15 D17:D22">
     <cfRule type="dataBar" priority="40">
@@ -4607,6 +4775,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0"/>

</xml_diff>

<commit_message>
Added a data dictionary.
</commit_message>
<xml_diff>
--- a/Documentation/Gantt Chart.xlsx
+++ b/Documentation/Gantt Chart.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9DA341A-719F-4820-8FBF-03319A49157B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{762C1B49-6A51-41FC-A536-C73FF683FAB1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="7125" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectSchedule" sheetId="11" r:id="rId1"/>
@@ -1706,109 +1706,6 @@
     <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="4" borderId="54" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="4" borderId="52" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="4" borderId="55" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="4" borderId="51" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="4" borderId="53" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="47" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="31" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="45" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="56" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="57" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="47" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="45" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="10" fontId="27" fillId="6" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="58" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="59" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="27" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="169" fontId="7" fillId="3" borderId="24" xfId="10" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1888,6 +1785,109 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="69" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="27" fillId="6" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="45" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="58" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="59" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="45" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="56" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="57" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="47" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="4" borderId="54" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="4" borderId="52" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="4" borderId="53" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="47" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="31" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="9" fontId="27" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="4" borderId="55" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="4" borderId="51" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="14">
@@ -2581,9 +2581,8 @@
   </sheetPr>
   <dimension ref="A1:BQ25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A11" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2601,11 +2600,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:69" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="AU1" s="144"/>
-      <c r="AV1" s="144"/>
-      <c r="AW1" s="144"/>
-      <c r="AX1" s="144"/>
-      <c r="AY1" s="144"/>
+      <c r="AU1" s="109"/>
+      <c r="AV1" s="109"/>
+      <c r="AW1" s="109"/>
+      <c r="AX1" s="109"/>
+      <c r="AY1" s="109"/>
     </row>
     <row r="2" spans="1:69" ht="24.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="26" t="s">
@@ -2630,11 +2629,11 @@
       <c r="AN2" t="s">
         <v>38</v>
       </c>
-      <c r="AU2" s="144"/>
-      <c r="AV2" s="144"/>
-      <c r="AW2" s="145"/>
-      <c r="AX2" s="145"/>
-      <c r="AY2" s="144"/>
+      <c r="AU2" s="109"/>
+      <c r="AV2" s="109"/>
+      <c r="AW2" s="110"/>
+      <c r="AX2" s="110"/>
+      <c r="AY2" s="109"/>
     </row>
     <row r="3" spans="1:69" ht="3" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="26"/>
@@ -2647,11 +2646,11 @@
       <c r="I3" s="10"/>
       <c r="AL3" s="37"/>
       <c r="AM3" s="32"/>
-      <c r="AU3" s="144"/>
-      <c r="AV3" s="144"/>
-      <c r="AW3" s="145"/>
-      <c r="AX3" s="145"/>
-      <c r="AY3" s="144"/>
+      <c r="AU3" s="109"/>
+      <c r="AV3" s="109"/>
+      <c r="AW3" s="110"/>
+      <c r="AX3" s="110"/>
+      <c r="AY3" s="109"/>
     </row>
     <row r="4" spans="1:69" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="25" t="s">
@@ -2665,14 +2664,14 @@
       </c>
       <c r="D4" s="104">
         <f ca="1">D5-F4</f>
-        <v>-0.45503144654088046</v>
+        <v>-0.24204545454545445</v>
       </c>
       <c r="E4" s="102" t="s">
         <v>53</v>
       </c>
       <c r="F4" s="103">
         <f ca="1">(60-D6)/60</f>
-        <v>0.98333333333333328</v>
+        <v>1</v>
       </c>
       <c r="I4" s="28" t="s">
         <v>15</v>
@@ -2682,11 +2681,11 @@
       <c r="AN4" t="s">
         <v>39</v>
       </c>
-      <c r="AU4" s="144"/>
-      <c r="AV4" s="144"/>
-      <c r="AW4" s="144"/>
-      <c r="AX4" s="144"/>
-      <c r="AY4" s="144"/>
+      <c r="AU4" s="109"/>
+      <c r="AV4" s="109"/>
+      <c r="AW4" s="109"/>
+      <c r="AX4" s="109"/>
+      <c r="AY4" s="109"/>
     </row>
     <row r="5" spans="1:69" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5"/>
@@ -2698,7 +2697,7 @@
       </c>
       <c r="D5" s="40">
         <f>SUM(D10,D15)/2</f>
-        <v>0.52830188679245282</v>
+        <v>0.75795454545454555</v>
       </c>
       <c r="E5" s="80" t="s">
         <v>0</v>
@@ -2707,8 +2706,8 @@
         <f>DATE(2020, 6, 15)</f>
         <v>43997</v>
       </c>
-      <c r="G5" s="108"/>
-      <c r="H5" s="108"/>
+      <c r="G5" s="166"/>
+      <c r="H5" s="166"/>
     </row>
     <row r="6" spans="1:69" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A6"/>
@@ -2720,7 +2719,7 @@
       </c>
       <c r="D6" s="41">
         <f ca="1">DATEDIF(NOW(),BP7,"D")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6" s="80" t="s">
         <v>6</v>
@@ -2728,107 +2727,107 @@
       <c r="F6" s="82">
         <v>1</v>
       </c>
-      <c r="G6" s="108"/>
-      <c r="H6" s="108"/>
-      <c r="I6" s="109">
+      <c r="G6" s="166"/>
+      <c r="H6" s="166"/>
+      <c r="I6" s="167">
         <f>I7</f>
         <v>43997</v>
       </c>
-      <c r="J6" s="106"/>
-      <c r="K6" s="106"/>
-      <c r="L6" s="106"/>
-      <c r="M6" s="106"/>
-      <c r="N6" s="106"/>
-      <c r="O6" s="110"/>
-      <c r="P6" s="105">
+      <c r="J6" s="155"/>
+      <c r="K6" s="155"/>
+      <c r="L6" s="155"/>
+      <c r="M6" s="155"/>
+      <c r="N6" s="155"/>
+      <c r="O6" s="156"/>
+      <c r="P6" s="154">
         <f>P7</f>
         <v>44004</v>
       </c>
-      <c r="Q6" s="106"/>
-      <c r="R6" s="106"/>
-      <c r="S6" s="106"/>
-      <c r="T6" s="106"/>
-      <c r="U6" s="106"/>
-      <c r="V6" s="110"/>
-      <c r="W6" s="105">
+      <c r="Q6" s="155"/>
+      <c r="R6" s="155"/>
+      <c r="S6" s="155"/>
+      <c r="T6" s="155"/>
+      <c r="U6" s="155"/>
+      <c r="V6" s="156"/>
+      <c r="W6" s="154">
         <f>W7</f>
         <v>44011</v>
       </c>
-      <c r="X6" s="106"/>
-      <c r="Y6" s="106"/>
-      <c r="Z6" s="106"/>
-      <c r="AA6" s="106"/>
-      <c r="AB6" s="106"/>
-      <c r="AC6" s="110"/>
-      <c r="AD6" s="105">
+      <c r="X6" s="155"/>
+      <c r="Y6" s="155"/>
+      <c r="Z6" s="155"/>
+      <c r="AA6" s="155"/>
+      <c r="AB6" s="155"/>
+      <c r="AC6" s="156"/>
+      <c r="AD6" s="154">
         <f>AD7</f>
         <v>44018</v>
       </c>
-      <c r="AE6" s="106"/>
-      <c r="AF6" s="106"/>
-      <c r="AG6" s="106"/>
-      <c r="AH6" s="106"/>
-      <c r="AI6" s="106"/>
-      <c r="AJ6" s="110"/>
-      <c r="AK6" s="105">
+      <c r="AE6" s="155"/>
+      <c r="AF6" s="155"/>
+      <c r="AG6" s="155"/>
+      <c r="AH6" s="155"/>
+      <c r="AI6" s="155"/>
+      <c r="AJ6" s="156"/>
+      <c r="AK6" s="154">
         <f>AK7</f>
         <v>44025</v>
       </c>
-      <c r="AL6" s="106"/>
-      <c r="AM6" s="106"/>
-      <c r="AN6" s="106"/>
-      <c r="AO6" s="106"/>
-      <c r="AP6" s="106"/>
-      <c r="AQ6" s="110"/>
-      <c r="AR6" s="105">
+      <c r="AL6" s="155"/>
+      <c r="AM6" s="155"/>
+      <c r="AN6" s="155"/>
+      <c r="AO6" s="155"/>
+      <c r="AP6" s="155"/>
+      <c r="AQ6" s="156"/>
+      <c r="AR6" s="154">
         <f>AR7</f>
         <v>44032</v>
       </c>
-      <c r="AS6" s="106"/>
-      <c r="AT6" s="106"/>
-      <c r="AU6" s="106"/>
-      <c r="AV6" s="106"/>
-      <c r="AW6" s="106"/>
-      <c r="AX6" s="110"/>
-      <c r="AY6" s="105">
+      <c r="AS6" s="155"/>
+      <c r="AT6" s="155"/>
+      <c r="AU6" s="155"/>
+      <c r="AV6" s="155"/>
+      <c r="AW6" s="155"/>
+      <c r="AX6" s="156"/>
+      <c r="AY6" s="154">
         <f>AY7</f>
         <v>44039</v>
       </c>
-      <c r="AZ6" s="106"/>
-      <c r="BA6" s="106"/>
-      <c r="BB6" s="106"/>
-      <c r="BC6" s="106"/>
-      <c r="BD6" s="106"/>
-      <c r="BE6" s="110"/>
-      <c r="BF6" s="105">
+      <c r="AZ6" s="155"/>
+      <c r="BA6" s="155"/>
+      <c r="BB6" s="155"/>
+      <c r="BC6" s="155"/>
+      <c r="BD6" s="155"/>
+      <c r="BE6" s="156"/>
+      <c r="BF6" s="154">
         <f>BF7</f>
         <v>44046</v>
       </c>
-      <c r="BG6" s="106"/>
-      <c r="BH6" s="106"/>
-      <c r="BI6" s="106"/>
-      <c r="BJ6" s="106"/>
-      <c r="BK6" s="106"/>
-      <c r="BL6" s="110"/>
-      <c r="BM6" s="105">
+      <c r="BG6" s="155"/>
+      <c r="BH6" s="155"/>
+      <c r="BI6" s="155"/>
+      <c r="BJ6" s="155"/>
+      <c r="BK6" s="155"/>
+      <c r="BL6" s="156"/>
+      <c r="BM6" s="154">
         <f>BM7</f>
         <v>44053</v>
       </c>
-      <c r="BN6" s="106"/>
-      <c r="BO6" s="106"/>
-      <c r="BP6" s="106"/>
-      <c r="BQ6" s="107"/>
+      <c r="BN6" s="155"/>
+      <c r="BO6" s="155"/>
+      <c r="BP6" s="155"/>
+      <c r="BQ6" s="165"/>
     </row>
     <row r="7" spans="1:69" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="115"/>
-      <c r="C7" s="115"/>
-      <c r="D7" s="115"/>
-      <c r="E7" s="115"/>
-      <c r="F7" s="115"/>
-      <c r="G7" s="115"/>
+      <c r="B7" s="157"/>
+      <c r="C7" s="157"/>
+      <c r="D7" s="157"/>
+      <c r="E7" s="157"/>
+      <c r="F7" s="157"/>
+      <c r="G7" s="157"/>
       <c r="I7" s="100">
         <f>Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
         <v>43997</v>
@@ -3091,10 +3090,10 @@
       <c r="F8" s="99" t="s">
         <v>4</v>
       </c>
-      <c r="G8" s="118" t="s">
+      <c r="G8" s="160" t="s">
         <v>5</v>
       </c>
-      <c r="H8" s="119"/>
+      <c r="H8" s="161"/>
       <c r="I8" s="9" t="str">
         <f>LEFT(TEXT(I7,"ddd"),1)</f>
         <v>M</v>
@@ -3423,14 +3422,14 @@
       <c r="C10" s="66"/>
       <c r="D10" s="78">
         <f>(D12*DATEDIF(E12,F12,"D")+D13*DATEDIF(E13,F13,"D")+D14*DATEDIF(E14,F14,"D"))/(DATEDIF(E12,F12,"D")+DATEDIF(E13,F13,"D")+DATEDIF(E14,F14,"D"))</f>
-        <v>0.55000000000000004</v>
+        <v>0.8</v>
       </c>
       <c r="E10" s="67"/>
       <c r="F10" s="68"/>
-      <c r="G10" s="139">
+      <c r="G10" s="164">
         <v>1</v>
       </c>
-      <c r="H10" s="139"/>
+      <c r="H10" s="164"/>
       <c r="I10" s="68"/>
       <c r="J10" s="68"/>
       <c r="K10" s="68"/>
@@ -3495,12 +3494,11 @@
     </row>
     <row r="11" spans="1:69" s="3" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="25"/>
-      <c r="B11" s="133" t="s">
+      <c r="B11" s="138" t="s">
         <v>42</v>
       </c>
-      <c r="C11" s="134"/>
+      <c r="C11" s="139"/>
       <c r="D11" s="62">
-        <f ca="1">(60-DATEDIF(NOW(),F11,"D"))/59</f>
         <v>1</v>
       </c>
       <c r="E11" s="70">
@@ -3511,11 +3509,11 @@
         <f>E11+59</f>
         <v>44056</v>
       </c>
-      <c r="G11" s="135">
+      <c r="G11" s="140">
         <f t="shared" ref="G11:G22" si="4">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v>60</v>
       </c>
-      <c r="H11" s="136"/>
+      <c r="H11" s="141"/>
       <c r="I11" s="63"/>
       <c r="J11" s="64"/>
       <c r="K11" s="64"/>
@@ -3582,10 +3580,10 @@
       <c r="A12" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="128" t="s">
+      <c r="B12" s="136" t="s">
         <v>52</v>
       </c>
-      <c r="C12" s="129"/>
+      <c r="C12" s="137"/>
       <c r="D12" s="12">
         <v>0.2</v>
       </c>
@@ -3595,15 +3593,15 @@
       <c r="F12" s="74">
         <v>44056</v>
       </c>
-      <c r="G12" s="137">
+      <c r="G12" s="142">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="H12" s="138"/>
+      <c r="H12" s="143"/>
       <c r="I12" s="47"/>
       <c r="J12" s="33"/>
-      <c r="K12" s="142"/>
-      <c r="L12" s="143"/>
+      <c r="K12" s="107"/>
+      <c r="L12" s="108"/>
       <c r="M12" s="33"/>
       <c r="N12" s="33"/>
       <c r="O12" s="33"/>
@@ -3666,12 +3664,12 @@
       <c r="A13" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="128" t="s">
+      <c r="B13" s="136" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="129"/>
+      <c r="C13" s="137"/>
       <c r="D13" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13" s="71">
         <v>44055</v>
@@ -3679,20 +3677,20 @@
       <c r="F13" s="74">
         <v>44056</v>
       </c>
-      <c r="G13" s="137">
+      <c r="G13" s="142">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="H13" s="138"/>
+      <c r="H13" s="143"/>
       <c r="I13" s="46"/>
       <c r="J13" s="33"/>
       <c r="K13" s="33"/>
       <c r="L13" s="33"/>
-      <c r="M13" s="146"/>
-      <c r="N13" s="147"/>
-      <c r="O13" s="147"/>
-      <c r="P13" s="147"/>
-      <c r="Q13" s="148"/>
+      <c r="M13" s="111"/>
+      <c r="N13" s="112"/>
+      <c r="O13" s="112"/>
+      <c r="P13" s="112"/>
+      <c r="Q13" s="113"/>
       <c r="R13" s="33"/>
       <c r="S13" s="33"/>
       <c r="T13" s="33"/>
@@ -3748,10 +3746,10 @@
     </row>
     <row r="14" spans="1:69" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="25"/>
-      <c r="B14" s="126" t="s">
+      <c r="B14" s="148" t="s">
         <v>41</v>
       </c>
-      <c r="C14" s="127"/>
+      <c r="C14" s="149"/>
       <c r="D14" s="49">
         <v>1</v>
       </c>
@@ -3761,21 +3759,21 @@
       <c r="F14" s="75">
         <v>44055</v>
       </c>
-      <c r="G14" s="131">
+      <c r="G14" s="134">
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
-      <c r="H14" s="132"/>
+      <c r="H14" s="135"/>
       <c r="I14" s="50"/>
       <c r="J14" s="51"/>
       <c r="K14" s="51"/>
       <c r="L14" s="51"/>
       <c r="M14" s="51"/>
       <c r="N14" s="51"/>
-      <c r="O14" s="149"/>
-      <c r="P14" s="150"/>
-      <c r="Q14" s="151"/>
-      <c r="R14" s="152"/>
+      <c r="O14" s="114"/>
+      <c r="P14" s="115"/>
+      <c r="Q14" s="116"/>
+      <c r="R14" s="117"/>
       <c r="S14" s="51"/>
       <c r="T14" s="51"/>
       <c r="U14" s="51"/>
@@ -3838,15 +3836,15 @@
       <c r="C15" s="55"/>
       <c r="D15" s="56">
         <f>(D16*DATEDIF(E16,F16,"D")+D17*DATEDIF(E17,F17,"D")+D18*DATEDIF(E18,F18,"D")+D19*DATEDIF(E19,F19,"D")+D20*DATEDIF(E20,F20,"D")+D21*DATEDIF(E21,F21,"D")+D22*DATEDIF(E22,F22,"D"))/(DATEDIF(E16,F16,"D")+DATEDIF(E17,F17,"D")+DATEDIF(E18,F18,"D")+DATEDIF(E19,F19,"D")+DATEDIF(E20,F20,"D")+DATEDIF(E21,F21,"D")+DATEDIF(E22,F22,"D"))</f>
-        <v>0.5066037735849056</v>
+        <v>0.71590909090909094</v>
       </c>
       <c r="E15" s="57"/>
       <c r="F15" s="58"/>
-      <c r="G15" s="130">
+      <c r="G15" s="133">
         <f ca="1">DATEDIF(E16,NOW(), "D")/DATEDIF(E16,BQ7,"d")</f>
-        <v>0.96610169491525422</v>
-      </c>
-      <c r="H15" s="130"/>
+        <v>0.98305084745762716</v>
+      </c>
+      <c r="H15" s="133"/>
       <c r="I15" s="59"/>
       <c r="J15" s="59"/>
       <c r="K15" s="59"/>
@@ -3856,8 +3854,8 @@
       <c r="O15" s="59"/>
       <c r="P15" s="59"/>
       <c r="Q15" s="59"/>
-      <c r="R15" s="154"/>
-      <c r="S15" s="154"/>
+      <c r="R15" s="119"/>
+      <c r="S15" s="119"/>
       <c r="T15" s="59"/>
       <c r="U15" s="59"/>
       <c r="V15" s="59"/>
@@ -3911,10 +3909,10 @@
     </row>
     <row r="16" spans="1:69" s="3" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="26"/>
-      <c r="B16" s="124" t="s">
+      <c r="B16" s="146" t="s">
         <v>49</v>
       </c>
-      <c r="C16" s="125"/>
+      <c r="C16" s="147"/>
       <c r="D16" s="52">
         <v>1</v>
       </c>
@@ -3925,11 +3923,11 @@
         <f>E16+1</f>
         <v>43999</v>
       </c>
-      <c r="G16" s="116">
+      <c r="G16" s="158">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="H16" s="117"/>
+      <c r="H16" s="159"/>
       <c r="I16" s="53"/>
       <c r="J16" s="54"/>
       <c r="K16" s="54"/>
@@ -3938,32 +3936,32 @@
       <c r="N16" s="54"/>
       <c r="O16" s="54"/>
       <c r="P16" s="54"/>
-      <c r="Q16" s="153"/>
-      <c r="R16" s="155"/>
-      <c r="S16" s="157"/>
-      <c r="T16" s="158"/>
-      <c r="U16" s="159"/>
-      <c r="V16" s="159"/>
-      <c r="W16" s="159"/>
-      <c r="X16" s="159"/>
+      <c r="Q16" s="118"/>
+      <c r="R16" s="120"/>
+      <c r="S16" s="122"/>
+      <c r="T16" s="123"/>
+      <c r="U16" s="124"/>
+      <c r="V16" s="124"/>
+      <c r="W16" s="124"/>
+      <c r="X16" s="124"/>
       <c r="Y16" s="44"/>
-      <c r="Z16" s="159"/>
-      <c r="AA16" s="159"/>
-      <c r="AB16" s="159"/>
-      <c r="AC16" s="159"/>
-      <c r="AD16" s="159"/>
-      <c r="AE16" s="159"/>
-      <c r="AF16" s="159"/>
-      <c r="AG16" s="159"/>
-      <c r="AH16" s="159"/>
-      <c r="AI16" s="159"/>
-      <c r="AJ16" s="159"/>
-      <c r="AK16" s="159"/>
-      <c r="AL16" s="159"/>
-      <c r="AM16" s="159"/>
-      <c r="AN16" s="159"/>
-      <c r="AO16" s="159"/>
-      <c r="AP16" s="159"/>
+      <c r="Z16" s="124"/>
+      <c r="AA16" s="124"/>
+      <c r="AB16" s="124"/>
+      <c r="AC16" s="124"/>
+      <c r="AD16" s="124"/>
+      <c r="AE16" s="124"/>
+      <c r="AF16" s="124"/>
+      <c r="AG16" s="124"/>
+      <c r="AH16" s="124"/>
+      <c r="AI16" s="124"/>
+      <c r="AJ16" s="124"/>
+      <c r="AK16" s="124"/>
+      <c r="AL16" s="124"/>
+      <c r="AM16" s="124"/>
+      <c r="AN16" s="124"/>
+      <c r="AO16" s="124"/>
+      <c r="AP16" s="124"/>
       <c r="AQ16" s="54"/>
       <c r="AR16" s="54"/>
       <c r="AS16" s="54"/>
@@ -3994,12 +3992,12 @@
     </row>
     <row r="17" spans="1:69" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="26"/>
-      <c r="B17" s="122" t="s">
+      <c r="B17" s="144" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="123"/>
+      <c r="C17" s="145"/>
       <c r="D17" s="13">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="E17" s="77">
         <v>44033</v>
@@ -4007,11 +4005,11 @@
       <c r="F17" s="77">
         <v>44056</v>
       </c>
-      <c r="G17" s="111">
+      <c r="G17" s="150">
         <f t="shared" si="4"/>
         <v>24</v>
       </c>
-      <c r="H17" s="112"/>
+      <c r="H17" s="151"/>
       <c r="I17" s="48"/>
       <c r="J17" s="35"/>
       <c r="K17" s="35"/>
@@ -4021,34 +4019,34 @@
       <c r="O17" s="35"/>
       <c r="P17" s="35"/>
       <c r="Q17" s="35"/>
-      <c r="R17" s="153"/>
-      <c r="S17" s="155"/>
-      <c r="T17" s="160"/>
-      <c r="U17" s="160"/>
-      <c r="V17" s="160"/>
-      <c r="W17" s="160"/>
-      <c r="X17" s="160"/>
-      <c r="Y17" s="161"/>
-      <c r="Z17" s="160"/>
-      <c r="AA17" s="160"/>
-      <c r="AB17" s="160"/>
-      <c r="AC17" s="160"/>
-      <c r="AD17" s="160"/>
-      <c r="AE17" s="160"/>
-      <c r="AF17" s="160"/>
-      <c r="AG17" s="160"/>
-      <c r="AH17" s="162"/>
-      <c r="AI17" s="162"/>
-      <c r="AJ17" s="162"/>
-      <c r="AK17" s="162"/>
-      <c r="AL17" s="162"/>
-      <c r="AM17" s="162"/>
-      <c r="AN17" s="162"/>
-      <c r="AO17" s="162"/>
-      <c r="AP17" s="157"/>
-      <c r="AQ17" s="163"/>
-      <c r="AR17" s="164"/>
-      <c r="AS17" s="164"/>
+      <c r="R17" s="118"/>
+      <c r="S17" s="120"/>
+      <c r="T17" s="125"/>
+      <c r="U17" s="125"/>
+      <c r="V17" s="125"/>
+      <c r="W17" s="125"/>
+      <c r="X17" s="125"/>
+      <c r="Y17" s="126"/>
+      <c r="Z17" s="125"/>
+      <c r="AA17" s="125"/>
+      <c r="AB17" s="125"/>
+      <c r="AC17" s="125"/>
+      <c r="AD17" s="125"/>
+      <c r="AE17" s="125"/>
+      <c r="AF17" s="125"/>
+      <c r="AG17" s="125"/>
+      <c r="AH17" s="127"/>
+      <c r="AI17" s="127"/>
+      <c r="AJ17" s="127"/>
+      <c r="AK17" s="127"/>
+      <c r="AL17" s="127"/>
+      <c r="AM17" s="127"/>
+      <c r="AN17" s="127"/>
+      <c r="AO17" s="127"/>
+      <c r="AP17" s="122"/>
+      <c r="AQ17" s="128"/>
+      <c r="AR17" s="129"/>
+      <c r="AS17" s="129"/>
       <c r="AT17" s="35"/>
       <c r="AU17" s="35"/>
       <c r="AV17" s="35"/>
@@ -4076,12 +4074,12 @@
     </row>
     <row r="18" spans="1:69" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="25"/>
-      <c r="B18" s="122" t="s">
+      <c r="B18" s="144" t="s">
         <v>45</v>
       </c>
-      <c r="C18" s="123"/>
+      <c r="C18" s="145"/>
       <c r="D18" s="13">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E18" s="77">
         <f>F17-7</f>
@@ -4091,11 +4089,11 @@
         <f>E18+7</f>
         <v>44056</v>
       </c>
-      <c r="G18" s="111">
+      <c r="G18" s="150">
         <f t="shared" si="4"/>
         <v>8</v>
       </c>
-      <c r="H18" s="112"/>
+      <c r="H18" s="151"/>
       <c r="I18" s="48"/>
       <c r="J18" s="35"/>
       <c r="K18" s="35"/>
@@ -4120,24 +4118,24 @@
       <c r="AD18" s="54"/>
       <c r="AE18" s="54"/>
       <c r="AF18" s="54"/>
-      <c r="AG18" s="153"/>
-      <c r="AH18" s="155"/>
-      <c r="AI18" s="160"/>
-      <c r="AJ18" s="160"/>
-      <c r="AK18" s="160"/>
-      <c r="AL18" s="160"/>
-      <c r="AM18" s="160"/>
-      <c r="AN18" s="160"/>
-      <c r="AO18" s="162"/>
-      <c r="AP18" s="162"/>
-      <c r="AQ18" s="162"/>
-      <c r="AR18" s="162"/>
-      <c r="AS18" s="157"/>
-      <c r="AT18" s="163"/>
-      <c r="AU18" s="164"/>
-      <c r="AV18" s="164"/>
-      <c r="AW18" s="164"/>
-      <c r="AX18" s="164"/>
+      <c r="AG18" s="118"/>
+      <c r="AH18" s="120"/>
+      <c r="AI18" s="125"/>
+      <c r="AJ18" s="125"/>
+      <c r="AK18" s="125"/>
+      <c r="AL18" s="125"/>
+      <c r="AM18" s="125"/>
+      <c r="AN18" s="125"/>
+      <c r="AO18" s="127"/>
+      <c r="AP18" s="127"/>
+      <c r="AQ18" s="127"/>
+      <c r="AR18" s="127"/>
+      <c r="AS18" s="122"/>
+      <c r="AT18" s="128"/>
+      <c r="AU18" s="129"/>
+      <c r="AV18" s="129"/>
+      <c r="AW18" s="129"/>
+      <c r="AX18" s="129"/>
       <c r="AY18" s="35"/>
       <c r="AZ18" s="35"/>
       <c r="BA18" s="35"/>
@@ -4160,26 +4158,24 @@
     </row>
     <row r="19" spans="1:69" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="25"/>
-      <c r="B19" s="122" t="s">
+      <c r="B19" s="144" t="s">
         <v>44</v>
       </c>
-      <c r="C19" s="123"/>
+      <c r="C19" s="145"/>
       <c r="D19" s="13">
         <v>0</v>
       </c>
       <c r="E19" s="77">
-        <f>F17-7</f>
-        <v>44049</v>
+        <v>44055</v>
       </c>
       <c r="F19" s="77">
-        <f>E19+10</f>
-        <v>44059</v>
-      </c>
-      <c r="G19" s="111">
+        <v>44056</v>
+      </c>
+      <c r="G19" s="150">
         <f t="shared" si="4"/>
-        <v>11</v>
-      </c>
-      <c r="H19" s="112"/>
+        <v>2</v>
+      </c>
+      <c r="H19" s="151"/>
       <c r="I19" s="48"/>
       <c r="J19" s="35"/>
       <c r="K19" s="35"/>
@@ -4211,19 +4207,19 @@
       <c r="AK19" s="54"/>
       <c r="AL19" s="54"/>
       <c r="AM19" s="54"/>
-      <c r="AN19" s="153"/>
-      <c r="AO19" s="155"/>
-      <c r="AP19" s="160"/>
-      <c r="AQ19" s="160"/>
-      <c r="AR19" s="160"/>
-      <c r="AS19" s="160"/>
-      <c r="AT19" s="160"/>
-      <c r="AU19" s="160"/>
-      <c r="AV19" s="160"/>
-      <c r="AW19" s="162"/>
-      <c r="AX19" s="157"/>
-      <c r="AY19" s="163"/>
-      <c r="AZ19" s="164"/>
+      <c r="AN19" s="118"/>
+      <c r="AO19" s="120"/>
+      <c r="AP19" s="125"/>
+      <c r="AQ19" s="125"/>
+      <c r="AR19" s="125"/>
+      <c r="AS19" s="125"/>
+      <c r="AT19" s="125"/>
+      <c r="AU19" s="125"/>
+      <c r="AV19" s="125"/>
+      <c r="AW19" s="127"/>
+      <c r="AX19" s="122"/>
+      <c r="AY19" s="128"/>
+      <c r="AZ19" s="129"/>
       <c r="BA19" s="35"/>
       <c r="BB19" s="35"/>
       <c r="BC19" s="35"/>
@@ -4244,26 +4240,26 @@
     </row>
     <row r="20" spans="1:69" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="25"/>
-      <c r="B20" s="122" t="s">
+      <c r="B20" s="144" t="s">
         <v>48</v>
       </c>
-      <c r="C20" s="123"/>
+      <c r="C20" s="145"/>
       <c r="D20" s="13">
         <v>0</v>
       </c>
       <c r="E20" s="77">
         <f>F19-3</f>
-        <v>44056</v>
+        <v>44053</v>
       </c>
       <c r="F20" s="77">
         <f>E20+10</f>
-        <v>44066</v>
-      </c>
-      <c r="G20" s="111">
+        <v>44063</v>
+      </c>
+      <c r="G20" s="150">
         <f t="shared" si="4"/>
         <v>11</v>
       </c>
-      <c r="H20" s="112"/>
+      <c r="H20" s="151"/>
       <c r="I20" s="48"/>
       <c r="J20" s="35"/>
       <c r="K20" s="35"/>
@@ -4295,23 +4291,23 @@
       <c r="AK20" s="35"/>
       <c r="AL20" s="35"/>
       <c r="AM20" s="35"/>
-      <c r="AN20" s="164"/>
-      <c r="AO20" s="159"/>
-      <c r="AP20" s="159"/>
+      <c r="AN20" s="129"/>
+      <c r="AO20" s="124"/>
+      <c r="AP20" s="124"/>
       <c r="AQ20" s="54"/>
       <c r="AR20" s="54"/>
       <c r="AS20" s="54"/>
       <c r="AT20" s="54"/>
       <c r="AU20" s="54"/>
-      <c r="AV20" s="153"/>
-      <c r="AW20" s="155"/>
-      <c r="AX20" s="160"/>
-      <c r="AY20" s="162"/>
-      <c r="AZ20" s="157"/>
-      <c r="BA20" s="163"/>
-      <c r="BB20" s="164"/>
-      <c r="BC20" s="164"/>
-      <c r="BD20" s="164"/>
+      <c r="AV20" s="118"/>
+      <c r="AW20" s="120"/>
+      <c r="AX20" s="125"/>
+      <c r="AY20" s="127"/>
+      <c r="AZ20" s="122"/>
+      <c r="BA20" s="128"/>
+      <c r="BB20" s="129"/>
+      <c r="BC20" s="129"/>
+      <c r="BD20" s="129"/>
       <c r="BE20" s="35"/>
       <c r="BF20" s="35"/>
       <c r="BG20" s="35"/>
@@ -4328,24 +4324,24 @@
     </row>
     <row r="21" spans="1:69" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="25"/>
-      <c r="B21" s="122" t="s">
+      <c r="B21" s="144" t="s">
         <v>47</v>
       </c>
-      <c r="C21" s="123"/>
+      <c r="C21" s="145"/>
       <c r="D21" s="13">
         <v>0.5</v>
       </c>
-      <c r="E21" s="140">
+      <c r="E21" s="105">
         <v>44055</v>
       </c>
-      <c r="F21" s="141">
+      <c r="F21" s="106">
         <v>44056</v>
       </c>
-      <c r="G21" s="111">
+      <c r="G21" s="150">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="H21" s="112"/>
+      <c r="H21" s="151"/>
       <c r="I21" s="48"/>
       <c r="J21" s="35"/>
       <c r="K21" s="35"/>
@@ -4376,10 +4372,10 @@
       <c r="AJ21" s="35"/>
       <c r="AK21" s="35"/>
       <c r="AL21" s="35"/>
-      <c r="AM21" s="166"/>
-      <c r="AN21" s="155"/>
-      <c r="AO21" s="160"/>
-      <c r="AP21" s="156"/>
+      <c r="AM21" s="131"/>
+      <c r="AN21" s="120"/>
+      <c r="AO21" s="125"/>
+      <c r="AP21" s="121"/>
       <c r="AQ21" s="48"/>
       <c r="AR21" s="35"/>
       <c r="AS21" s="35"/>
@@ -4387,17 +4383,17 @@
       <c r="AU21" s="35"/>
       <c r="AV21" s="35"/>
       <c r="AW21" s="54"/>
-      <c r="AX21" s="153"/>
-      <c r="AY21" s="155"/>
-      <c r="AZ21" s="160"/>
-      <c r="BA21" s="160"/>
-      <c r="BB21" s="160"/>
-      <c r="BC21" s="160"/>
-      <c r="BD21" s="157"/>
-      <c r="BE21" s="163"/>
-      <c r="BF21" s="164"/>
-      <c r="BG21" s="164"/>
-      <c r="BH21" s="164"/>
+      <c r="AX21" s="118"/>
+      <c r="AY21" s="120"/>
+      <c r="AZ21" s="125"/>
+      <c r="BA21" s="125"/>
+      <c r="BB21" s="125"/>
+      <c r="BC21" s="125"/>
+      <c r="BD21" s="122"/>
+      <c r="BE21" s="128"/>
+      <c r="BF21" s="129"/>
+      <c r="BG21" s="129"/>
+      <c r="BH21" s="129"/>
       <c r="BI21" s="35"/>
       <c r="BJ21" s="35"/>
       <c r="BK21" s="35"/>
@@ -4410,24 +4406,24 @@
     </row>
     <row r="22" spans="1:69" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="25"/>
-      <c r="B22" s="120" t="s">
+      <c r="B22" s="162" t="s">
         <v>46</v>
       </c>
-      <c r="C22" s="121"/>
+      <c r="C22" s="163"/>
       <c r="D22" s="83">
         <v>0</v>
       </c>
-      <c r="E22" s="140">
+      <c r="E22" s="105">
         <v>44055</v>
       </c>
-      <c r="F22" s="141">
+      <c r="F22" s="106">
         <v>44056</v>
       </c>
-      <c r="G22" s="113">
+      <c r="G22" s="152">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="H22" s="114"/>
+      <c r="H22" s="153"/>
       <c r="I22" s="84"/>
       <c r="J22" s="85"/>
       <c r="K22" s="85"/>
@@ -4459,9 +4455,9 @@
       <c r="AK22" s="85"/>
       <c r="AL22" s="85"/>
       <c r="AM22" s="85"/>
-      <c r="AN22" s="165"/>
-      <c r="AO22" s="165"/>
-      <c r="AP22" s="165"/>
+      <c r="AN22" s="130"/>
+      <c r="AO22" s="130"/>
+      <c r="AP22" s="130"/>
       <c r="AQ22" s="85"/>
       <c r="AR22" s="85"/>
       <c r="AS22" s="85"/>
@@ -4470,16 +4466,16 @@
       <c r="AV22" s="85"/>
       <c r="AW22" s="85"/>
       <c r="AX22" s="85"/>
-      <c r="AY22" s="165"/>
-      <c r="AZ22" s="165"/>
-      <c r="BA22" s="165"/>
-      <c r="BB22" s="165"/>
-      <c r="BC22" s="167"/>
-      <c r="BD22" s="155"/>
-      <c r="BE22" s="160"/>
-      <c r="BF22" s="160"/>
-      <c r="BG22" s="160"/>
-      <c r="BH22" s="156"/>
+      <c r="AY22" s="130"/>
+      <c r="AZ22" s="130"/>
+      <c r="BA22" s="130"/>
+      <c r="BB22" s="130"/>
+      <c r="BC22" s="132"/>
+      <c r="BD22" s="120"/>
+      <c r="BE22" s="125"/>
+      <c r="BF22" s="125"/>
+      <c r="BG22" s="125"/>
+      <c r="BH22" s="121"/>
       <c r="BI22" s="84"/>
       <c r="BJ22" s="85"/>
       <c r="BK22" s="85"/>
@@ -4502,18 +4498,14 @@
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="BM6:BQ6"/>
+    <mergeCell ref="G5:H6"/>
+    <mergeCell ref="I6:O6"/>
+    <mergeCell ref="P6:V6"/>
+    <mergeCell ref="W6:AC6"/>
+    <mergeCell ref="AD6:AJ6"/>
+    <mergeCell ref="AK6:AQ6"/>
     <mergeCell ref="G21:H21"/>
     <mergeCell ref="G22:H22"/>
     <mergeCell ref="AR6:AX6"/>
@@ -4530,14 +4522,18 @@
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="B19:C19"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="BM6:BQ6"/>
-    <mergeCell ref="G5:H6"/>
-    <mergeCell ref="I6:O6"/>
-    <mergeCell ref="P6:V6"/>
-    <mergeCell ref="W6:AC6"/>
-    <mergeCell ref="AD6:AJ6"/>
-    <mergeCell ref="AK6:AQ6"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="G13:H13"/>
   </mergeCells>
   <conditionalFormatting sqref="AF10:AF11 BH10:BH11 D9:D15 D17:D22">
     <cfRule type="dataBar" priority="40">

</xml_diff>

<commit_message>
2nd last update to the gantt chart.
</commit_message>
<xml_diff>
--- a/Documentation/Gantt Chart.xlsx
+++ b/Documentation/Gantt Chart.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{762C1B49-6A51-41FC-A536-C73FF683FAB1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50B02557-D807-4CD5-8797-8E5F97A2BE58}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -202,9 +202,6 @@
     <t>Lib. BASIC Code</t>
   </si>
   <si>
-    <t>Explain Modules</t>
-  </si>
-  <si>
     <t>Test Data</t>
   </si>
   <si>
@@ -233,6 +230,9 @@
   </si>
   <si>
     <t>Ahead/Behind:</t>
+  </si>
+  <si>
+    <t>Logbook</t>
   </si>
 </sst>
 </file>
@@ -541,7 +541,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="70">
+  <borders count="71">
     <border>
       <left/>
       <right/>
@@ -1382,6 +1382,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="dashed">
+        <color theme="0" tint="-0.1498764000366222"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </top>
+      <bottom style="medium">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1414,7 +1427,7 @@
     </xf>
     <xf numFmtId="0" fontId="26" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="168">
+  <cellXfs count="169">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1888,6 +1901,9 @@
     </xf>
     <xf numFmtId="167" fontId="0" fillId="4" borderId="51" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="70" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="14">
@@ -2581,8 +2597,8 @@
   </sheetPr>
   <dimension ref="A1:BQ25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A11" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="F11" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2660,14 +2676,14 @@
         <v>34</v>
       </c>
       <c r="C4" s="38" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D4" s="104">
         <f ca="1">D5-F4</f>
-        <v>-0.24204545454545445</v>
+        <v>-1.388888888888884E-2</v>
       </c>
       <c r="E4" s="102" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F4" s="103">
         <f ca="1">(60-D6)/60</f>
@@ -2693,11 +2709,11 @@
         <v>25</v>
       </c>
       <c r="C5" s="39" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D5" s="40">
         <f>SUM(D10,D15)/2</f>
-        <v>0.75795454545454555</v>
+        <v>0.98611111111111116</v>
       </c>
       <c r="E5" s="80" t="s">
         <v>0</v>
@@ -2715,7 +2731,7 @@
         <v>26</v>
       </c>
       <c r="C6" s="38" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D6" s="41">
         <f ca="1">DATEDIF(NOW(),BP7,"D")</f>
@@ -3422,7 +3438,7 @@
       <c r="C10" s="66"/>
       <c r="D10" s="78">
         <f>(D12*DATEDIF(E12,F12,"D")+D13*DATEDIF(E13,F13,"D")+D14*DATEDIF(E14,F14,"D"))/(DATEDIF(E12,F12,"D")+DATEDIF(E13,F13,"D")+DATEDIF(E14,F14,"D"))</f>
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="E10" s="67"/>
       <c r="F10" s="68"/>
@@ -3581,11 +3597,11 @@
         <v>30</v>
       </c>
       <c r="B12" s="136" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C12" s="137"/>
       <c r="D12" s="12">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="E12" s="71">
         <v>44055</v>
@@ -3836,7 +3852,7 @@
       <c r="C15" s="55"/>
       <c r="D15" s="56">
         <f>(D16*DATEDIF(E16,F16,"D")+D17*DATEDIF(E17,F17,"D")+D18*DATEDIF(E18,F18,"D")+D19*DATEDIF(E19,F19,"D")+D20*DATEDIF(E20,F20,"D")+D21*DATEDIF(E21,F21,"D")+D22*DATEDIF(E22,F22,"D"))/(DATEDIF(E16,F16,"D")+DATEDIF(E17,F17,"D")+DATEDIF(E18,F18,"D")+DATEDIF(E19,F19,"D")+DATEDIF(E20,F20,"D")+DATEDIF(E21,F21,"D")+DATEDIF(E22,F22,"D"))</f>
-        <v>0.71590909090909094</v>
+        <v>0.97222222222222221</v>
       </c>
       <c r="E15" s="57"/>
       <c r="F15" s="58"/>
@@ -3910,7 +3926,7 @@
     <row r="16" spans="1:69" s="3" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="26"/>
       <c r="B16" s="146" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C16" s="147"/>
       <c r="D16" s="52">
@@ -4075,7 +4091,7 @@
     <row r="18" spans="1:69" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="25"/>
       <c r="B18" s="144" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C18" s="145"/>
       <c r="D18" s="13">
@@ -4159,11 +4175,11 @@
     <row r="19" spans="1:69" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="25"/>
       <c r="B19" s="144" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="C19" s="145"/>
       <c r="D19" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19" s="77">
         <v>44055</v>
@@ -4171,10 +4187,7 @@
       <c r="F19" s="77">
         <v>44056</v>
       </c>
-      <c r="G19" s="150">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
+      <c r="G19" s="168"/>
       <c r="H19" s="151"/>
       <c r="I19" s="48"/>
       <c r="J19" s="35"/>
@@ -4241,23 +4254,21 @@
     <row r="20" spans="1:69" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="25"/>
       <c r="B20" s="144" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C20" s="145"/>
       <c r="D20" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E20" s="77">
-        <f>F19-3</f>
-        <v>44053</v>
+        <v>44054</v>
       </c>
       <c r="F20" s="77">
-        <f>E20+10</f>
-        <v>44063</v>
+        <v>44056</v>
       </c>
       <c r="G20" s="150">
         <f t="shared" si="4"/>
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="H20" s="151"/>
       <c r="I20" s="48"/>
@@ -4325,11 +4336,11 @@
     <row r="21" spans="1:69" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="25"/>
       <c r="B21" s="144" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C21" s="145"/>
       <c r="D21" s="13">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E21" s="105">
         <v>44055</v>
@@ -4407,17 +4418,17 @@
     <row r="22" spans="1:69" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="25"/>
       <c r="B22" s="162" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C22" s="163"/>
       <c r="D22" s="83">
         <v>0</v>
       </c>
       <c r="E22" s="105">
-        <v>44055</v>
+        <v>44056</v>
       </c>
       <c r="F22" s="106">
-        <v>44056</v>
+        <v>44057</v>
       </c>
       <c r="G22" s="152">
         <f t="shared" si="4"/>

</xml_diff>

<commit_message>
Final changes to readme.md, excluding evaluation.
</commit_message>
<xml_diff>
--- a/Documentation/Gantt Chart.xlsx
+++ b/Documentation/Gantt Chart.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50B02557-D807-4CD5-8797-8E5F97A2BE58}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{237AA8E3-D56E-4A63-AEF9-5791A33FBBD3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1799,14 +1799,78 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="69" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="27" fillId="6" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="9" fontId="27" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="4" borderId="54" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="4" borderId="52" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="4" borderId="55" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="4" borderId="51" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="4" borderId="53" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="70" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="47" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="31" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="45" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="56" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="57" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="47" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="45" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
@@ -1814,6 +1878,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="58" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
@@ -1832,77 +1902,7 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="45" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="56" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="57" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="47" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="4" borderId="54" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="4" borderId="52" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="4" borderId="53" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="47" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="31" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="9" fontId="27" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="4" borderId="55" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="4" borderId="51" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="70" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="27" fillId="6" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2597,8 +2597,8 @@
   </sheetPr>
   <dimension ref="A1:BQ25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="F11" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A6" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2679,14 +2679,14 @@
         <v>53</v>
       </c>
       <c r="D4" s="104">
-        <f ca="1">D5-F4</f>
+        <f>D5-F4</f>
         <v>-1.388888888888884E-2</v>
       </c>
       <c r="E4" s="102" t="s">
         <v>52</v>
       </c>
       <c r="F4" s="103">
-        <f ca="1">(60-D6)/60</f>
+        <f>(60-D6)/60</f>
         <v>1</v>
       </c>
       <c r="I4" s="28" t="s">
@@ -2722,8 +2722,8 @@
         <f>DATE(2020, 6, 15)</f>
         <v>43997</v>
       </c>
-      <c r="G5" s="166"/>
-      <c r="H5" s="166"/>
+      <c r="G5" s="137"/>
+      <c r="H5" s="137"/>
     </row>
     <row r="6" spans="1:69" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A6"/>
@@ -2734,7 +2734,6 @@
         <v>50</v>
       </c>
       <c r="D6" s="41">
-        <f ca="1">DATEDIF(NOW(),BP7,"D")</f>
         <v>0</v>
       </c>
       <c r="E6" s="80" t="s">
@@ -2743,107 +2742,107 @@
       <c r="F6" s="82">
         <v>1</v>
       </c>
-      <c r="G6" s="166"/>
-      <c r="H6" s="166"/>
-      <c r="I6" s="167">
+      <c r="G6" s="137"/>
+      <c r="H6" s="137"/>
+      <c r="I6" s="138">
         <f>I7</f>
         <v>43997</v>
       </c>
-      <c r="J6" s="155"/>
-      <c r="K6" s="155"/>
-      <c r="L6" s="155"/>
-      <c r="M6" s="155"/>
-      <c r="N6" s="155"/>
-      <c r="O6" s="156"/>
-      <c r="P6" s="154">
+      <c r="J6" s="135"/>
+      <c r="K6" s="135"/>
+      <c r="L6" s="135"/>
+      <c r="M6" s="135"/>
+      <c r="N6" s="135"/>
+      <c r="O6" s="139"/>
+      <c r="P6" s="134">
         <f>P7</f>
         <v>44004</v>
       </c>
-      <c r="Q6" s="155"/>
-      <c r="R6" s="155"/>
-      <c r="S6" s="155"/>
-      <c r="T6" s="155"/>
-      <c r="U6" s="155"/>
-      <c r="V6" s="156"/>
-      <c r="W6" s="154">
+      <c r="Q6" s="135"/>
+      <c r="R6" s="135"/>
+      <c r="S6" s="135"/>
+      <c r="T6" s="135"/>
+      <c r="U6" s="135"/>
+      <c r="V6" s="139"/>
+      <c r="W6" s="134">
         <f>W7</f>
         <v>44011</v>
       </c>
-      <c r="X6" s="155"/>
-      <c r="Y6" s="155"/>
-      <c r="Z6" s="155"/>
-      <c r="AA6" s="155"/>
-      <c r="AB6" s="155"/>
-      <c r="AC6" s="156"/>
-      <c r="AD6" s="154">
+      <c r="X6" s="135"/>
+      <c r="Y6" s="135"/>
+      <c r="Z6" s="135"/>
+      <c r="AA6" s="135"/>
+      <c r="AB6" s="135"/>
+      <c r="AC6" s="139"/>
+      <c r="AD6" s="134">
         <f>AD7</f>
         <v>44018</v>
       </c>
-      <c r="AE6" s="155"/>
-      <c r="AF6" s="155"/>
-      <c r="AG6" s="155"/>
-      <c r="AH6" s="155"/>
-      <c r="AI6" s="155"/>
-      <c r="AJ6" s="156"/>
-      <c r="AK6" s="154">
+      <c r="AE6" s="135"/>
+      <c r="AF6" s="135"/>
+      <c r="AG6" s="135"/>
+      <c r="AH6" s="135"/>
+      <c r="AI6" s="135"/>
+      <c r="AJ6" s="139"/>
+      <c r="AK6" s="134">
         <f>AK7</f>
         <v>44025</v>
       </c>
-      <c r="AL6" s="155"/>
-      <c r="AM6" s="155"/>
-      <c r="AN6" s="155"/>
-      <c r="AO6" s="155"/>
-      <c r="AP6" s="155"/>
-      <c r="AQ6" s="156"/>
-      <c r="AR6" s="154">
+      <c r="AL6" s="135"/>
+      <c r="AM6" s="135"/>
+      <c r="AN6" s="135"/>
+      <c r="AO6" s="135"/>
+      <c r="AP6" s="135"/>
+      <c r="AQ6" s="139"/>
+      <c r="AR6" s="134">
         <f>AR7</f>
         <v>44032</v>
       </c>
-      <c r="AS6" s="155"/>
-      <c r="AT6" s="155"/>
-      <c r="AU6" s="155"/>
-      <c r="AV6" s="155"/>
-      <c r="AW6" s="155"/>
-      <c r="AX6" s="156"/>
-      <c r="AY6" s="154">
+      <c r="AS6" s="135"/>
+      <c r="AT6" s="135"/>
+      <c r="AU6" s="135"/>
+      <c r="AV6" s="135"/>
+      <c r="AW6" s="135"/>
+      <c r="AX6" s="139"/>
+      <c r="AY6" s="134">
         <f>AY7</f>
         <v>44039</v>
       </c>
-      <c r="AZ6" s="155"/>
-      <c r="BA6" s="155"/>
-      <c r="BB6" s="155"/>
-      <c r="BC6" s="155"/>
-      <c r="BD6" s="155"/>
-      <c r="BE6" s="156"/>
-      <c r="BF6" s="154">
+      <c r="AZ6" s="135"/>
+      <c r="BA6" s="135"/>
+      <c r="BB6" s="135"/>
+      <c r="BC6" s="135"/>
+      <c r="BD6" s="135"/>
+      <c r="BE6" s="139"/>
+      <c r="BF6" s="134">
         <f>BF7</f>
         <v>44046</v>
       </c>
-      <c r="BG6" s="155"/>
-      <c r="BH6" s="155"/>
-      <c r="BI6" s="155"/>
-      <c r="BJ6" s="155"/>
-      <c r="BK6" s="155"/>
-      <c r="BL6" s="156"/>
-      <c r="BM6" s="154">
+      <c r="BG6" s="135"/>
+      <c r="BH6" s="135"/>
+      <c r="BI6" s="135"/>
+      <c r="BJ6" s="135"/>
+      <c r="BK6" s="135"/>
+      <c r="BL6" s="139"/>
+      <c r="BM6" s="134">
         <f>BM7</f>
         <v>44053</v>
       </c>
-      <c r="BN6" s="155"/>
-      <c r="BO6" s="155"/>
-      <c r="BP6" s="155"/>
-      <c r="BQ6" s="165"/>
+      <c r="BN6" s="135"/>
+      <c r="BO6" s="135"/>
+      <c r="BP6" s="135"/>
+      <c r="BQ6" s="136"/>
     </row>
     <row r="7" spans="1:69" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="157"/>
-      <c r="C7" s="157"/>
-      <c r="D7" s="157"/>
-      <c r="E7" s="157"/>
-      <c r="F7" s="157"/>
-      <c r="G7" s="157"/>
+      <c r="B7" s="144"/>
+      <c r="C7" s="144"/>
+      <c r="D7" s="144"/>
+      <c r="E7" s="144"/>
+      <c r="F7" s="144"/>
+      <c r="G7" s="144"/>
       <c r="I7" s="100">
         <f>Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
         <v>43997</v>
@@ -3106,10 +3105,10 @@
       <c r="F8" s="99" t="s">
         <v>4</v>
       </c>
-      <c r="G8" s="160" t="s">
+      <c r="G8" s="148" t="s">
         <v>5</v>
       </c>
-      <c r="H8" s="161"/>
+      <c r="H8" s="149"/>
       <c r="I8" s="9" t="str">
         <f>LEFT(TEXT(I7,"ddd"),1)</f>
         <v>M</v>
@@ -3442,10 +3441,10 @@
       </c>
       <c r="E10" s="67"/>
       <c r="F10" s="68"/>
-      <c r="G10" s="164">
+      <c r="G10" s="133">
         <v>1</v>
       </c>
-      <c r="H10" s="164"/>
+      <c r="H10" s="133"/>
       <c r="I10" s="68"/>
       <c r="J10" s="68"/>
       <c r="K10" s="68"/>
@@ -3510,10 +3509,10 @@
     </row>
     <row r="11" spans="1:69" s="3" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="25"/>
-      <c r="B11" s="138" t="s">
+      <c r="B11" s="162" t="s">
         <v>42</v>
       </c>
-      <c r="C11" s="139"/>
+      <c r="C11" s="163"/>
       <c r="D11" s="62">
         <v>1</v>
       </c>
@@ -3525,11 +3524,11 @@
         <f>E11+59</f>
         <v>44056</v>
       </c>
-      <c r="G11" s="140">
+      <c r="G11" s="164">
         <f t="shared" ref="G11:G22" si="4">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v>60</v>
       </c>
-      <c r="H11" s="141"/>
+      <c r="H11" s="165"/>
       <c r="I11" s="63"/>
       <c r="J11" s="64"/>
       <c r="K11" s="64"/>
@@ -3596,10 +3595,10 @@
       <c r="A12" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="136" t="s">
+      <c r="B12" s="158" t="s">
         <v>51</v>
       </c>
-      <c r="C12" s="137"/>
+      <c r="C12" s="159"/>
       <c r="D12" s="12">
         <v>1</v>
       </c>
@@ -3609,11 +3608,11 @@
       <c r="F12" s="74">
         <v>44056</v>
       </c>
-      <c r="G12" s="142">
+      <c r="G12" s="166">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="H12" s="143"/>
+      <c r="H12" s="167"/>
       <c r="I12" s="47"/>
       <c r="J12" s="33"/>
       <c r="K12" s="107"/>
@@ -3680,10 +3679,10 @@
       <c r="A13" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="136" t="s">
+      <c r="B13" s="158" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="137"/>
+      <c r="C13" s="159"/>
       <c r="D13" s="12">
         <v>1</v>
       </c>
@@ -3693,11 +3692,11 @@
       <c r="F13" s="74">
         <v>44056</v>
       </c>
-      <c r="G13" s="142">
+      <c r="G13" s="166">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="H13" s="143"/>
+      <c r="H13" s="167"/>
       <c r="I13" s="46"/>
       <c r="J13" s="33"/>
       <c r="K13" s="33"/>
@@ -3762,10 +3761,10 @@
     </row>
     <row r="14" spans="1:69" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="25"/>
-      <c r="B14" s="148" t="s">
+      <c r="B14" s="156" t="s">
         <v>41</v>
       </c>
-      <c r="C14" s="149"/>
+      <c r="C14" s="157"/>
       <c r="D14" s="49">
         <v>1</v>
       </c>
@@ -3775,11 +3774,11 @@
       <c r="F14" s="75">
         <v>44055</v>
       </c>
-      <c r="G14" s="134">
+      <c r="G14" s="160">
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
-      <c r="H14" s="135"/>
+      <c r="H14" s="161"/>
       <c r="I14" s="50"/>
       <c r="J14" s="51"/>
       <c r="K14" s="51"/>
@@ -3856,11 +3855,10 @@
       </c>
       <c r="E15" s="57"/>
       <c r="F15" s="58"/>
-      <c r="G15" s="133">
-        <f ca="1">DATEDIF(E16,NOW(), "D")/DATEDIF(E16,BQ7,"d")</f>
-        <v>0.98305084745762716</v>
-      </c>
-      <c r="H15" s="133"/>
+      <c r="G15" s="168">
+        <v>1</v>
+      </c>
+      <c r="H15" s="168"/>
       <c r="I15" s="59"/>
       <c r="J15" s="59"/>
       <c r="K15" s="59"/>
@@ -3925,10 +3923,10 @@
     </row>
     <row r="16" spans="1:69" s="3" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="26"/>
-      <c r="B16" s="146" t="s">
+      <c r="B16" s="154" t="s">
         <v>48</v>
       </c>
-      <c r="C16" s="147"/>
+      <c r="C16" s="155"/>
       <c r="D16" s="52">
         <v>1</v>
       </c>
@@ -3939,11 +3937,11 @@
         <f>E16+1</f>
         <v>43999</v>
       </c>
-      <c r="G16" s="158">
+      <c r="G16" s="145">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="H16" s="159"/>
+      <c r="H16" s="146"/>
       <c r="I16" s="53"/>
       <c r="J16" s="54"/>
       <c r="K16" s="54"/>
@@ -4008,10 +4006,10 @@
     </row>
     <row r="17" spans="1:69" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="26"/>
-      <c r="B17" s="144" t="s">
+      <c r="B17" s="152" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="145"/>
+      <c r="C17" s="153"/>
       <c r="D17" s="13">
         <v>1</v>
       </c>
@@ -4021,11 +4019,11 @@
       <c r="F17" s="77">
         <v>44056</v>
       </c>
-      <c r="G17" s="150">
+      <c r="G17" s="140">
         <f t="shared" si="4"/>
         <v>24</v>
       </c>
-      <c r="H17" s="151"/>
+      <c r="H17" s="141"/>
       <c r="I17" s="48"/>
       <c r="J17" s="35"/>
       <c r="K17" s="35"/>
@@ -4090,10 +4088,10 @@
     </row>
     <row r="18" spans="1:69" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="25"/>
-      <c r="B18" s="144" t="s">
+      <c r="B18" s="152" t="s">
         <v>44</v>
       </c>
-      <c r="C18" s="145"/>
+      <c r="C18" s="153"/>
       <c r="D18" s="13">
         <v>1</v>
       </c>
@@ -4105,11 +4103,11 @@
         <f>E18+7</f>
         <v>44056</v>
       </c>
-      <c r="G18" s="150">
+      <c r="G18" s="140">
         <f t="shared" si="4"/>
         <v>8</v>
       </c>
-      <c r="H18" s="151"/>
+      <c r="H18" s="141"/>
       <c r="I18" s="48"/>
       <c r="J18" s="35"/>
       <c r="K18" s="35"/>
@@ -4174,10 +4172,10 @@
     </row>
     <row r="19" spans="1:69" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="25"/>
-      <c r="B19" s="144" t="s">
+      <c r="B19" s="152" t="s">
         <v>54</v>
       </c>
-      <c r="C19" s="145"/>
+      <c r="C19" s="153"/>
       <c r="D19" s="13">
         <v>1</v>
       </c>
@@ -4187,8 +4185,10 @@
       <c r="F19" s="77">
         <v>44056</v>
       </c>
-      <c r="G19" s="168"/>
-      <c r="H19" s="151"/>
+      <c r="G19" s="147">
+        <v>1</v>
+      </c>
+      <c r="H19" s="141"/>
       <c r="I19" s="48"/>
       <c r="J19" s="35"/>
       <c r="K19" s="35"/>
@@ -4253,10 +4253,10 @@
     </row>
     <row r="20" spans="1:69" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="25"/>
-      <c r="B20" s="144" t="s">
+      <c r="B20" s="152" t="s">
         <v>47</v>
       </c>
-      <c r="C20" s="145"/>
+      <c r="C20" s="153"/>
       <c r="D20" s="13">
         <v>1</v>
       </c>
@@ -4266,11 +4266,11 @@
       <c r="F20" s="77">
         <v>44056</v>
       </c>
-      <c r="G20" s="150">
+      <c r="G20" s="140">
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
-      <c r="H20" s="151"/>
+      <c r="H20" s="141"/>
       <c r="I20" s="48"/>
       <c r="J20" s="35"/>
       <c r="K20" s="35"/>
@@ -4335,10 +4335,10 @@
     </row>
     <row r="21" spans="1:69" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="25"/>
-      <c r="B21" s="144" t="s">
+      <c r="B21" s="152" t="s">
         <v>46</v>
       </c>
-      <c r="C21" s="145"/>
+      <c r="C21" s="153"/>
       <c r="D21" s="13">
         <v>1</v>
       </c>
@@ -4348,11 +4348,11 @@
       <c r="F21" s="106">
         <v>44056</v>
       </c>
-      <c r="G21" s="150">
+      <c r="G21" s="140">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="H21" s="151"/>
+      <c r="H21" s="141"/>
       <c r="I21" s="48"/>
       <c r="J21" s="35"/>
       <c r="K21" s="35"/>
@@ -4417,10 +4417,10 @@
     </row>
     <row r="22" spans="1:69" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="25"/>
-      <c r="B22" s="162" t="s">
+      <c r="B22" s="150" t="s">
         <v>45</v>
       </c>
-      <c r="C22" s="163"/>
+      <c r="C22" s="151"/>
       <c r="D22" s="83">
         <v>0</v>
       </c>
@@ -4430,11 +4430,11 @@
       <c r="F22" s="106">
         <v>44057</v>
       </c>
-      <c r="G22" s="152">
+      <c r="G22" s="142">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="H22" s="153"/>
+      <c r="H22" s="143"/>
       <c r="I22" s="84"/>
       <c r="J22" s="85"/>
       <c r="K22" s="85"/>
@@ -4509,14 +4509,18 @@
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="BM6:BQ6"/>
-    <mergeCell ref="G5:H6"/>
-    <mergeCell ref="I6:O6"/>
-    <mergeCell ref="P6:V6"/>
-    <mergeCell ref="W6:AC6"/>
-    <mergeCell ref="AD6:AJ6"/>
-    <mergeCell ref="AK6:AQ6"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B13:C13"/>
     <mergeCell ref="G21:H21"/>
     <mergeCell ref="G22:H22"/>
     <mergeCell ref="AR6:AX6"/>
@@ -4533,18 +4537,14 @@
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="BM6:BQ6"/>
+    <mergeCell ref="G5:H6"/>
+    <mergeCell ref="I6:O6"/>
+    <mergeCell ref="P6:V6"/>
+    <mergeCell ref="W6:AC6"/>
+    <mergeCell ref="AD6:AJ6"/>
+    <mergeCell ref="AK6:AQ6"/>
   </mergeCells>
   <conditionalFormatting sqref="AF10:AF11 BH10:BH11 D9:D15 D17:D22">
     <cfRule type="dataBar" priority="40">

</xml_diff>